<commit_message>
Matching whole word instead of substring & Chart phase done
- Added utility to check for whole word so expected value matching is
on whole word rather than substrings
- Chart phase done
</commit_message>
<xml_diff>
--- a/auto-agent/workflow.xlsx
+++ b/auto-agent/workflow.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="181">
   <si>
     <t>So, what do you think? Overall do you think {{.TargetFactor.FactorName}} makes a difference to performance in space?</t>
   </si>
@@ -52,18 +52,9 @@
     <t xml:space="preserve">                  "Id": "chart conclusion"</t>
   </si>
   <si>
-    <t xml:space="preserve">                                "Id": "chart conclusion"</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                  "Id": "chart conclusion"</t>
   </si>
   <si>
-    <t xml:space="preserve">                                "Id": "memo"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                              "Id": "chart correct non-causal conclusion"</t>
-  </si>
-  <si>
     <t xml:space="preserve">                      "Id": "chart wrong non-causal conclusion"</t>
   </si>
   <si>
@@ -79,9 +70,6 @@
     <t xml:space="preserve">                                "Id": "chart correct causal explain step by step"</t>
   </si>
   <si>
-    <t xml:space="preserve">                              "Id": "chart conclusion"</t>
-  </si>
-  <si>
     <t xml:space="preserve">                    "Id": "chart non-causal"</t>
   </si>
   <si>
@@ -124,9 +112,6 @@
     <t>I see.</t>
   </si>
   <si>
-    <t>Ok, got it. So you think that {{.TargetFactor.FactorName}} really does not make a difference to performance. Now, suppose someone disagrees with you and thinks that {{.TargetFactor.FactorName}} does make a difference to performance in space, what would you say to them?</t>
-  </si>
-  <si>
     <t>Ok. Now, let's look again at the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}}, what are the best and worst performance for these people? And what about the people who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}}? what are the best and worst performance for those people?</t>
   </si>
   <si>
@@ -169,15 +154,6 @@
     <t>Ok. So it seems that having different levels for {{.TargetFactor.FactorName}} give you different performance.</t>
   </si>
   <si>
-    <t>I see. Now, how do you think the chart would look different if {{.TargetFactor.FactorName}} does make a difference to performance?</t>
-  </si>
-  <si>
-    <t>Ok, let me make sure I got that. Let's look at the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}}, what are the best and worst performance for these people? And what about the people who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}}? what are the best and worst performance for those people?</t>
-  </si>
-  <si>
-    <t>Ok, no problem. Let's see if we can figure it out together. Let's look at the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}}, what are the best and worst performance for these people? And what about the people who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}}? what are the best and worst performance for those people?</t>
-  </si>
-  <si>
     <t>So, what do you think? What does this tell you about whether {{.TargetFactor.FactorName}} makes a difference to performance?</t>
   </si>
   <si>
@@ -196,9 +172,6 @@
     <t>So, what do you think? Overall do you think {{.TargetFactor.FactorName}} makes a difference to performance?</t>
   </si>
   <si>
-    <t>makes a difference?</t>
-  </si>
-  <si>
     <t>Ok. I see. So for {{.TargetFactor.FactorName}}, which level do you think is best to have for performance?</t>
   </si>
   <si>
@@ -256,30 +229,12 @@
     <t>correct. see any differences?</t>
   </si>
   <si>
-    <t>non-causal. someone disagree.</t>
-  </si>
-  <si>
-    <t>correct. best and worst performance?</t>
-  </si>
-  <si>
     <t>hint. is there best level? best level?</t>
   </si>
   <si>
     <t>hint. have different performance.</t>
   </si>
   <si>
-    <t>help</t>
-  </si>
-  <si>
-    <t>wrong</t>
-  </si>
-  <si>
-    <t>correct</t>
-  </si>
-  <si>
-    <t>hint</t>
-  </si>
-  <si>
     <t>record. see chart. makes a difference?</t>
   </si>
   <si>
@@ -406,18 +361,6 @@
     <t xml:space="preserve">                                "Id": "chart wrong non-causal different levels"</t>
   </si>
   <si>
-    <t xml:space="preserve">                            "Id": "chart correct non-causal conclusion"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                              "Id": "chart correct non-causal challenge"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                            "Id": "chart correct non-causal conclusion see difference"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                            "Id": "chart correct non-causal explain not sure"</t>
-  </si>
-  <si>
     <t xml:space="preserve">                "Id": "chart non-causal refers to chart"</t>
   </si>
   <si>
@@ -478,9 +421,6 @@
     <t>non-causal.correct.Q_someone_disagree.1</t>
   </si>
   <si>
-    <t>??Add</t>
-  </si>
-  <si>
     <t>non-causal.Q_why.2</t>
   </si>
   <si>
@@ -599,6 +539,30 @@
   </si>
   <si>
     <t>non-causal.assume_chart.2</t>
+  </si>
+  <si>
+    <t>non-causal.wrong.help.correct.MC_is_causal.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                "Id": "chart wrong non-causal correct best leve chart conclusion"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  "Id": "chart not sure"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  "Id": "chart wrong non-causal conclusion"</t>
+  </si>
+  <si>
+    <t>non-causal.wrong.help.correct.wrong.Q_best_worst.2.1.2</t>
+  </si>
+  <si>
+    <t>Ok. Now, Let's look at the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}} for {{.TargetFactor.FactorName}}, what are the best and worst performance for these people? And what about the people who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}}? what are the best and worst performance for those people?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    "Id": "chart conclusion step by step"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                  "Id": "chart correct causal explain step by step double check"</t>
   </si>
 </sst>
 </file>
@@ -630,7 +594,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,6 +703,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -749,7 +731,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="979">
+  <cellStyleXfs count="1149">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1729,8 +1711,178 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -1750,10 +1902,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="979">
+  <cellStyles count="1149">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2243,6 +2397,91 @@
     <cellStyle name="Followed Hyperlink" xfId="974" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="976" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="978" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="980" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="982" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="984" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="986" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="988" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="990" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="992" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="994" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="996" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="998" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1000" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1002" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1004" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1006" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1008" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1010" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1012" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1014" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1016" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1018" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1020" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1022" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1024" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1026" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1028" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1030" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1032" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1034" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1036" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1038" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1040" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1042" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1044" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1046" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1048" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1050" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1052" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1054" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1056" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1058" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1060" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1062" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1064" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1066" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1068" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1070" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1072" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1074" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1076" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1078" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1080" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1082" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1084" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1086" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1088" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1090" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1092" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1094" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1096" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1098" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1148" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2732,6 +2971,91 @@
     <cellStyle name="Hyperlink" xfId="973" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="975" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="977" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="979" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="981" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="983" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="985" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="987" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="989" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="991" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="993" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="995" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="997" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="999" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1001" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1003" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1005" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1007" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1009" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1011" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1013" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1015" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1017" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1019" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1021" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1023" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1025" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1027" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1029" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1031" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1033" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1035" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1037" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1039" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1041" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1043" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1045" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1047" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1049" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1051" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1053" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1055" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1057" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1059" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1061" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1063" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1065" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1067" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1069" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1071" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1073" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1075" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1077" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1079" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1081" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1083" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1085" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1087" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1089" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1091" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1093" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1095" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1097" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1099" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1147" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3061,10 +3385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3073,1131 +3397,822 @@
     <col min="2" max="2" width="52.1640625" style="16" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.5" style="18" customWidth="1"/>
     <col min="6" max="6" width="21.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="B2" s="16" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:6">
       <c r="A5" s="15" t="s">
-        <v>107</v>
+        <v>92</v>
       </c>
       <c r="B5" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
         <v>93</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="B6" s="16" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>141</v>
+      </c>
+      <c r="C11" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="D11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" t="s">
+        <v>151</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" customFormat="1">
+      <c r="A17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" customFormat="1">
+      <c r="A18" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B18" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="C18" s="18"/>
+    </row>
+    <row r="19" spans="1:4" customFormat="1">
+      <c r="A19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>144</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="16" customFormat="1">
+      <c r="A20" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>159</v>
+      </c>
+      <c r="C20" s="18"/>
+    </row>
+    <row r="21" spans="1:4" s="16" customFormat="1">
+      <c r="A21" t="s">
+        <v>157</v>
+      </c>
+      <c r="B21" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" s="18"/>
+    </row>
+    <row r="22" spans="1:4" s="16" customFormat="1">
+      <c r="A22" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="18"/>
+    </row>
+    <row r="23" spans="1:4" customFormat="1">
+      <c r="A23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="18"/>
+    </row>
+    <row r="24" spans="1:4" customFormat="1">
+      <c r="A24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="18"/>
+    </row>
+    <row r="25" spans="1:4" customFormat="1">
+      <c r="A25" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="B25" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" customFormat="1">
+      <c r="A26" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B26" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C26" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="D5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>146</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B8" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
-        <v>110</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C9" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" s="5" t="s">
-        <v>112</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" customFormat="1">
+      <c r="A27" t="s">
+        <v>104</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D27" t="s">
         <v>32</v>
       </c>
-      <c r="E11" t="s">
-        <v>0</v>
-      </c>
-      <c r="G11" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D12" t="s">
+    </row>
+    <row r="28" spans="1:4" customFormat="1">
+      <c r="A28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B28" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C28" s="18"/>
+      <c r="D28" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
-        <v>114</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G15" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>116</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="16" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" s="16" customFormat="1">
-      <c r="C24" s="18"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" s="13" t="s">
-        <v>117</v>
-      </c>
-      <c r="B25" s="16" t="s">
-        <v>140</v>
-      </c>
-      <c r="C25" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="D25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B26" s="16" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" t="s">
-        <v>59</v>
-      </c>
-      <c r="H26" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>119</v>
-      </c>
-      <c r="B27" s="16" t="s">
-        <v>142</v>
-      </c>
-      <c r="C27" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="D27" t="s">
-        <v>37</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8">
-      <c r="A28" t="s">
-        <v>120</v>
-      </c>
-      <c r="B28" s="16" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:4" customFormat="1">
       <c r="A29" s="9" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>191</v>
-      </c>
+        <v>171</v>
+      </c>
+      <c r="C29" s="18"/>
       <c r="D29" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" customFormat="1">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>144</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="C30" s="18"/>
       <c r="D30" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" customFormat="1">
       <c r="A31" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="C31" s="18" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
-      </c>
-      <c r="H31" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" customFormat="1">
       <c r="A32" s="8" t="s">
         <v>7</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" s="16" customFormat="1">
-      <c r="C33" s="18"/>
-    </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C32" s="18"/>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B33" s="16" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="11" t="s">
+        <v>13</v>
+      </c>
       <c r="B34" s="16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="11" t="s">
-        <v>16</v>
+        <v>80</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" t="s">
+        <v>37</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" t="s">
+        <v>39</v>
+      </c>
+      <c r="F36" s="16" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="A37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B37" s="16" t="s">
+        <v>134</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="16" t="s">
+        <v>135</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" t="s">
+        <v>110</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>136</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="D39" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="B41" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="D42" s="16"/>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" s="16" t="s">
+        <v>177</v>
+      </c>
+      <c r="D43" s="16" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B44" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D44" s="16"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="B45" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" s="16"/>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" t="s">
         <v>42</v>
       </c>
-      <c r="E35" t="s">
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" s="16" customFormat="1">
-      <c r="C37" s="18"/>
-    </row>
-    <row r="38" spans="1:8">
-      <c r="A38" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="B38" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C38" s="18" t="s">
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="16" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" s="16" t="s">
+        <v>140</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" s="16" customFormat="1">
+      <c r="A50" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="B50" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="D50" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B51" s="16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="16" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="B53" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B54" s="16" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B55" s="16" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="21" t="s">
+        <v>114</v>
+      </c>
+      <c r="B57" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="22" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F59" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F38" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8">
-      <c r="A39" t="s">
-        <v>124</v>
-      </c>
-      <c r="B39" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8">
-      <c r="A40" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B40" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="D40" t="s">
-        <v>36</v>
-      </c>
-      <c r="H40" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8">
-      <c r="A41" t="s">
-        <v>125</v>
-      </c>
-      <c r="B41" s="16" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D41" t="s">
-        <v>46</v>
-      </c>
-      <c r="H41" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8">
-      <c r="A42" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="16" t="s">
-        <v>157</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>150</v>
-      </c>
-      <c r="D42" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8">
-      <c r="A43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B43" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8">
-      <c r="A44" t="s">
-        <v>126</v>
-      </c>
-      <c r="B44" s="16" t="s">
-        <v>158</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" t="s">
-        <v>47</v>
-      </c>
-      <c r="H44" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8">
-      <c r="A45" t="s">
-        <v>127</v>
-      </c>
-      <c r="B45" s="16" t="s">
-        <v>159</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="D45" t="s">
-        <v>48</v>
-      </c>
-      <c r="H45" s="16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B46" s="16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B47" s="16" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="D47" t="s">
-        <v>25</v>
-      </c>
-      <c r="H47" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" s="16" customFormat="1">
-      <c r="A48" s="16" t="s">
-        <v>152</v>
-      </c>
-      <c r="C48" s="18"/>
-    </row>
-    <row r="49" spans="1:8" s="16" customFormat="1">
-      <c r="A49" t="s">
-        <v>166</v>
-      </c>
-      <c r="B49" s="16" t="s">
-        <v>186</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="D49" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8">
-      <c r="A50" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="B50" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D50" t="s">
-        <v>31</v>
-      </c>
-      <c r="H50" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B51" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C51" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D51" t="s">
-        <v>32</v>
-      </c>
-      <c r="E51" t="s">
-        <v>0</v>
-      </c>
-      <c r="G51" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="B52" s="20" t="s">
-        <v>161</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="B53" s="20" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8">
-      <c r="A54" t="s">
-        <v>171</v>
-      </c>
-      <c r="B54" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="D54" t="s">
-        <v>27</v>
-      </c>
-      <c r="G54" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H54" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="B55" s="20" t="s">
-        <v>163</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D55" t="s">
-        <v>0</v>
-      </c>
-      <c r="G55" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="B56" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="B57" s="20" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="B58" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="D58" t="s">
-        <v>35</v>
-      </c>
-      <c r="H58" s="16" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="B59" s="20" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8">
-      <c r="A60" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60" s="20" t="s">
-        <v>164</v>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B60" s="16" t="s">
+        <v>79</v>
       </c>
       <c r="C60" s="18" t="s">
         <v>72</v>
       </c>
       <c r="D60" t="s">
-        <v>23</v>
-      </c>
-      <c r="H60" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" s="16" customFormat="1">
-      <c r="A61" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B61" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="C61" s="18"/>
-    </row>
-    <row r="62" spans="1:8" s="16" customFormat="1">
-      <c r="A62" t="s">
-        <v>177</v>
-      </c>
-      <c r="B62" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C62" s="18"/>
-    </row>
-    <row r="63" spans="1:8" s="16" customFormat="1">
-      <c r="A63" s="9" t="s">
-        <v>178</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B61" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B62" s="16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" s="11" t="s">
+        <v>163</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>191</v>
-      </c>
-      <c r="C63" s="18"/>
-    </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="20" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B65" s="20" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" s="16" customFormat="1">
-      <c r="C66" s="18"/>
-    </row>
-    <row r="67" spans="1:8" s="16" customFormat="1">
-      <c r="C67" s="18"/>
-    </row>
-    <row r="68" spans="1:8" s="16" customFormat="1">
-      <c r="C68" s="18"/>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B69" s="1"/>
+        <v>80</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D63" t="s">
+        <v>37</v>
+      </c>
+      <c r="E63" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B64" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
+      <c r="A65" t="s">
+        <v>118</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>167</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
+      <c r="A66" t="s">
+        <v>119</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="D66" t="s">
+        <v>20</v>
+      </c>
+      <c r="E66" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6">
+      <c r="A67" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6">
+      <c r="A68" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
+      <c r="A69" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>169</v>
+      </c>
       <c r="C69" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D69" t="s">
+        <v>48</v>
+      </c>
+      <c r="E69" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6">
+      <c r="A70" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B70" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="D69" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8">
-      <c r="A70" t="s">
-        <v>129</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="D70" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B71" s="1"/>
-    </row>
-    <row r="72" spans="1:8">
-      <c r="A72" t="s">
-        <v>130</v>
-      </c>
-      <c r="B72" s="1"/>
-      <c r="C72" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="D72" t="s">
-        <v>50</v>
-      </c>
-      <c r="H72" s="16" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B73" s="1"/>
-    </row>
-    <row r="74" spans="1:8">
-      <c r="A74" t="s">
-        <v>131</v>
-      </c>
-      <c r="B74" s="1"/>
-      <c r="C74" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D74" t="s">
-        <v>51</v>
-      </c>
-      <c r="H74" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B75" s="1"/>
-    </row>
-    <row r="76" spans="1:8" s="16" customFormat="1">
-      <c r="C76" s="18"/>
-    </row>
-    <row r="77" spans="1:8">
-      <c r="A77" t="s">
-        <v>132</v>
-      </c>
-      <c r="B77" s="16" t="s">
-        <v>192</v>
-      </c>
-      <c r="D77" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B78" s="16" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B79" s="16" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B80" s="16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" s="16" customFormat="1">
-      <c r="C81" s="18"/>
-    </row>
-    <row r="82" spans="1:8" s="16" customFormat="1">
-      <c r="C82" s="18"/>
-    </row>
-    <row r="83" spans="1:8">
-      <c r="A83" t="s">
+      <c r="C70" s="16"/>
+      <c r="F70"/>
+    </row>
+    <row r="71" spans="1:6">
+      <c r="A71" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B71" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="B83" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H83" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" t="s">
-        <v>134</v>
-      </c>
-      <c r="B84" s="16" t="s">
-        <v>182</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="D84" t="s">
-        <v>52</v>
-      </c>
-      <c r="G84" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" t="s">
-        <v>135</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="C85" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="D85" t="s">
-        <v>53</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B86" s="16" t="s">
-        <v>94</v>
-      </c>
-      <c r="C86" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D86" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B87" s="16" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B88" s="16" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="B89" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="C89" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="D89" t="s">
-        <v>42</v>
-      </c>
-      <c r="E89" t="s">
-        <v>43</v>
-      </c>
-      <c r="G89" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" s="16" customFormat="1">
-      <c r="C90" s="18"/>
-    </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B91" s="1"/>
-    </row>
-    <row r="92" spans="1:8" s="16" customFormat="1">
-      <c r="C92" s="18"/>
-    </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B93" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8">
-      <c r="A94" t="s">
-        <v>137</v>
-      </c>
-      <c r="B94" s="16" t="s">
-        <v>187</v>
-      </c>
-      <c r="C94" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="D94" t="s">
-        <v>54</v>
-      </c>
-      <c r="H94" s="16" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8">
-      <c r="A95" t="s">
-        <v>138</v>
-      </c>
-      <c r="B95" s="16" t="s">
-        <v>188</v>
-      </c>
-      <c r="C95" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="D95" t="s">
-        <v>24</v>
-      </c>
-      <c r="E95" t="s">
-        <v>55</v>
-      </c>
-      <c r="G95" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B96" s="16" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B97" s="16" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8">
-      <c r="A98" t="s">
-        <v>139</v>
-      </c>
-      <c r="B98" s="16" t="s">
-        <v>189</v>
-      </c>
-      <c r="C98" s="19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D98" t="s">
-        <v>56</v>
-      </c>
-      <c r="E98" t="s">
-        <v>57</v>
-      </c>
-      <c r="G98" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B99" s="16" t="s">
-        <v>93</v>
-      </c>
-      <c r="C99"/>
-      <c r="F99"/>
-      <c r="G99"/>
-      <c r="H99"/>
-    </row>
-    <row r="100" spans="1:8">
-      <c r="A100" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B100" s="16" t="s">
-        <v>153</v>
-      </c>
-      <c r="C100"/>
-      <c r="F100"/>
-      <c r="G100"/>
-      <c r="H100"/>
+      <c r="C71" s="16"/>
+      <c r="F71"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4228,100 +4243,100 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="7" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>167</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>98</v>
+        <v>147</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D2" s="20" t="s">
-        <v>185</v>
+        <v>148</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>171</v>
-      </c>
-      <c r="D3" s="20" t="s">
-        <v>162</v>
+        <v>151</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C4" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>163</v>
+        <v>152</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="20" t="s">
-        <v>96</v>
+        <v>153</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="17" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C6" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>161</v>
+        <v>154</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="17" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="C7" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>161</v>
+        <v>150</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -4329,27 +4344,27 @@
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>179</v>
+        <v>149</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="D9" s="20" t="s">
-        <v>97</v>
+        <v>145</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -4357,27 +4372,27 @@
         <v>2</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>185</v>
+        <v>148</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="C11" t="s">
-        <v>175</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>164</v>
+        <v>155</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -4385,29 +4400,29 @@
         <v>3</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>179</v>
+        <v>156</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="C13" t="s">
-        <v>177</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>180</v>
+        <v>157</v>
+      </c>
+      <c r="D13" s="19" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="C14" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>191</v>
+        <v>158</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chart phase summary in progress
</commit_message>
<xml_diff>
--- a/auto-agent/workflow.xlsx
+++ b/auto-agent/workflow.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="0" windowWidth="25660" windowHeight="14900" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2800" yWindow="120" windowWidth="23080" windowHeight="14800" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="workflowText.csv" sheetId="6" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="838" uniqueCount="377">
   <si>
     <t>So, what do you think? Overall do you think {{.TargetFactor.FactorName}} makes a difference to performance in space?</t>
   </si>
@@ -1043,9 +1043,6 @@
     <t>What you have selected seems to be different from your previous memos, let's look at some of the charts again together to refresh our memory.</t>
   </si>
   <si>
-    <t>Ok, remind me what made you decide that?</t>
-  </si>
-  <si>
     <t>correct</t>
   </si>
   <si>
@@ -1079,9 +1076,6 @@
     <t xml:space="preserve">    all_correct.Q_best_levels.2</t>
   </si>
   <si>
-    <t xml:space="preserve">        wrong.show_chart.MC_is_factor_causal.1</t>
-  </si>
-  <si>
     <t xml:space="preserve">                all_correct.Q_best_levels.2</t>
   </si>
   <si>
@@ -1091,55 +1085,73 @@
     <t xml:space="preserve">                wrong.wrong.MC_is_same_perf.1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">                    wrong.wrong.correct.1.2.2</t>
-  </si>
-  <si>
-    <t>I see. Let's look at this more carefully together.</t>
-  </si>
-  <si>
     <t>Look at the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}}, what are the best and worst performance for these people? And what about the people who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}}? what are the best and worst performance for those people?</t>
   </si>
   <si>
-    <t xml:space="preserve">                    wrong.wrong.wrong.Q_best_worst.1.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                        wrong.wrong.wrong.MC_is_causal.1.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                             wrong.wrong.wrong.correct.1.2.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                wrong.next_wrong_factor.1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                all_correct.Q_best_levels.2</t>
-  </si>
-  <si>
     <t>Ok, so you think that {{.TargetFactor.FactorName}} {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{if $factor.IsBeliefCausal}}makes{{else}}does not make{{end}} a difference to performance.</t>
   </si>
   <si>
-    <t xml:space="preserve">                                    wrong.wrong.wrong.MC_is_causal.1.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                             wrong.wrong.wrong.wrong.1.2.1.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                wrong.wrong.wrong.wrong.causal.1.2.1.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                wrong.wrong.wrong.wrong.non-causal.1.2.1.2.1</t>
-  </si>
-  <si>
     <t>Now, remember that when you look at the different levels of {{.TargetFactor.FactorName}} on the chart before, you noticed that those who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}}, their best performance was A but those who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}} did not get any A performance. So, you thought that having different levels for {{.TargetFactor.FactorName}} would give you different performance.</t>
   </si>
   <si>
     <t>Now, remember that when you look at the different levels of {{.TargetFactor.FactorName}} on the chart before, you noticed that the best was always A and the worst was always E for the levels? So, you thought that it didn't really matter which level to have for {{.TargetFactor.FactorName}}.</t>
   </si>
   <si>
-    <t>Great. So you found that {{$length := len .Beliefs.CausalFactors }}{{if eq $length 4}}all factors matter{{else if .Beliefs.CausalFactors}}{{range $i, $v := .Beliefs.CausalFactors}}{{if $i}}{{if eq $length 2}} and {{else if gt $i 1}} and {{else}}, {{end}}{{end}}{{$v}}{{end}}{{if .Beliefs.HasMultipleCausalFactors}} matter{{- else}} matters{{- end}}{{- else}}none of the factors matters{{- end}} to performance in space.</t>
-  </si>
-  <si>
-    <t>You’ve worked hard to figure out what factors mattered to the applicants’ performance. Now, you can use your knowledge to predict how well they will do. I have some new applicants here. Can you predict how well they will do? Then you can choose a best team of five.</t>
+    <t>Ok, looks like you have changed your mind on {{.TargetFactor.FactorName}}. That is fine. Now, tell me again, what made you decide that?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        wrong.wrong.wrong.MC_is_causal.1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    all_correct.Q_best_levels.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    wrong.next_wrong_factor.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    wrong.wrong.non-causal.1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        wrong.wrong.wrong.Q_best_worst.1.2.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                            wrong.wrong.wrong.MC_is_causal.1.2.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                wrong.wrong.wrong.correct.1.2.1.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                wrong.wrong.wrong.wrong.1.2.1.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    wrong.wrong.wrong.wrong.causal.1.2.1.1.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                    wrong.wrong.wrong.wrong.non-causal.1.2.1.1.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                    wrong.wrong.causal.1.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                        wrong.wrong.correct.1.2.1.2</t>
+  </si>
+  <si>
+    <t>Ok. Let's look at this more carefully together.</t>
+  </si>
+  <si>
+    <t>So you think that their performance would be the same.</t>
+  </si>
+  <si>
+    <t>So you think that their performance would be different.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        wrong.show_chart.MC_is_causal.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   wrong.show_chart.MC_is_causal.1</t>
+  </si>
+  <si>
+    <t>Great. Now you are ready for the next step. Press \"Enter\" to continue.</t>
   </si>
 </sst>
 </file>
@@ -1188,8 +1200,150 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1253">
+  <cellStyleXfs count="1395">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2446,7 +2600,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1253">
+  <cellStyles count="1395">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3073,6 +3227,77 @@
     <cellStyle name="Followed Hyperlink" xfId="1248" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1250" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1290" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1292" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1294" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1296" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1298" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1300" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1304" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1306" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1308" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1310" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1312" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1314" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1316" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1318" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1320" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1322" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1324" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1326" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1328" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1330" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1332" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1334" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1336" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1338" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1340" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1342" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1344" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1346" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1348" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1350" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1352" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1354" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1356" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1358" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1360" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1362" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1364" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1394" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -3699,6 +3924,77 @@
     <cellStyle name="Hyperlink" xfId="1247" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1249" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1289" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1291" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1293" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1295" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1297" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1299" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1303" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1305" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1307" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1309" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1311" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1313" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1315" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1317" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1319" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1321" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1323" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1325" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1327" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1329" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1331" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1333" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1335" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1337" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1339" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1341" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1343" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1345" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1347" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1349" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1351" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1353" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1355" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1357" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1359" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1361" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1363" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1393" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6626,275 +6922,264 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M130"/>
+  <dimension ref="A2:M136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <pane ySplit="2960" topLeftCell="A106" activePane="bottomLeft"/>
-      <selection activeCell="B84" sqref="B84"/>
-      <selection pane="bottomLeft" activeCell="M130" sqref="M130"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <pane ySplit="860" topLeftCell="A126" activePane="bottomLeft"/>
+      <selection activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="L136" sqref="L136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="9" width="4" customWidth="1"/>
-    <col min="10" max="10" width="39.83203125" customWidth="1"/>
+    <col min="10" max="10" width="26.83203125" customWidth="1"/>
     <col min="11" max="11" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
         <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L2" t="s">
-        <v>197</v>
-      </c>
-      <c r="M2" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>199</v>
-      </c>
-      <c r="K3" t="s">
-        <v>38</v>
+        <v>196</v>
       </c>
       <c r="L3" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="M3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K4" t="s">
         <v>38</v>
       </c>
       <c r="L4" t="s">
-        <v>203</v>
+        <v>200</v>
+      </c>
+      <c r="M4" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="K5" t="s">
         <v>38</v>
       </c>
       <c r="L5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="K6" t="s">
         <v>38</v>
+      </c>
+      <c r="L6" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="K7" t="s">
-        <v>208</v>
-      </c>
-      <c r="L7" t="s">
-        <v>209</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="K8" t="s">
-        <v>38</v>
+        <v>208</v>
+      </c>
+      <c r="L8" t="s">
+        <v>209</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K9" t="s">
-        <v>212</v>
-      </c>
-      <c r="L9" t="s">
-        <v>213</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="K10" t="s">
-        <v>38</v>
+        <v>212</v>
       </c>
       <c r="L10" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="K11" t="s">
         <v>38</v>
       </c>
       <c r="L11" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="K12" t="s">
         <v>38</v>
       </c>
       <c r="L12" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K13" t="s">
         <v>38</v>
       </c>
       <c r="L13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K14" t="s">
         <v>38</v>
+      </c>
+      <c r="L14" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="K15" t="s">
-        <v>223</v>
+        <v>38</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="K16" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="K17" t="s">
-        <v>227</v>
-      </c>
-      <c r="L17" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B18" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K18" t="s">
-        <v>38</v>
+        <v>227</v>
       </c>
       <c r="L18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K19" t="s">
         <v>38</v>
       </c>
       <c r="L19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="K20" t="s">
         <v>38</v>
+      </c>
+      <c r="L20" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="21" spans="1:13">
@@ -6902,376 +7187,376 @@
         <v>8</v>
       </c>
       <c r="B21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="K21" t="s">
-        <v>235</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B22" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="K22" t="s">
-        <v>223</v>
-      </c>
-      <c r="L22" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="K23" t="s">
-        <v>38</v>
+        <v>223</v>
       </c>
       <c r="L23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="K24" t="s">
         <v>38</v>
+      </c>
+      <c r="L24" t="s">
+        <v>239</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B25" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="K25" t="s">
-        <v>242</v>
-      </c>
-      <c r="L25" t="s">
-        <v>243</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K26" t="s">
-        <v>38</v>
+        <v>242</v>
       </c>
       <c r="L26" t="s">
-        <v>245</v>
-      </c>
-      <c r="M26" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B27" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="K27" t="s">
         <v>38</v>
       </c>
       <c r="L27" t="s">
-        <v>248</v>
+        <v>245</v>
+      </c>
+      <c r="M27" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="K28" t="s">
         <v>38</v>
+      </c>
+      <c r="L28" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K29" t="s">
-        <v>242</v>
-      </c>
-      <c r="L29" t="s">
-        <v>251</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B30" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="K30" t="s">
-        <v>38</v>
+        <v>242</v>
       </c>
       <c r="L30" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="K31" t="s">
         <v>38</v>
       </c>
       <c r="L31" t="s">
-        <v>255</v>
-      </c>
-      <c r="M31" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B32" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K32" t="s">
-        <v>258</v>
+        <v>38</v>
+      </c>
+      <c r="L32" t="s">
+        <v>255</v>
+      </c>
+      <c r="M32" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="K33" t="s">
-        <v>208</v>
-      </c>
-      <c r="L33" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="K34" t="s">
-        <v>38</v>
+        <v>208</v>
+      </c>
+      <c r="L34" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:13">
       <c r="A35">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="K35" t="s">
-        <v>263</v>
-      </c>
-      <c r="L35" t="s">
-        <v>264</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:13">
       <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="B36" t="s">
+        <v>262</v>
+      </c>
+      <c r="K36" t="s">
+        <v>263</v>
+      </c>
+      <c r="L36" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37">
         <v>8</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>240</v>
       </c>
-      <c r="K36" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13">
-      <c r="A38">
-        <v>0</v>
-      </c>
-      <c r="B38" t="s">
-        <v>52</v>
-      </c>
-      <c r="L38" t="s">
-        <v>53</v>
+      <c r="K37" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:13">
       <c r="A39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>265</v>
-      </c>
-      <c r="K39" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="L39" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
     </row>
     <row r="40" spans="1:13">
       <c r="A40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K40" t="s">
         <v>38</v>
       </c>
       <c r="L40" t="s">
-        <v>0</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:13">
       <c r="A41">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>267</v>
-      </c>
-      <c r="K41" t="b">
-        <v>1</v>
+        <v>266</v>
+      </c>
+      <c r="K41" t="s">
+        <v>38</v>
       </c>
       <c r="L41" t="s">
-        <v>22</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:13">
       <c r="A42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>268</v>
-      </c>
-      <c r="K42" t="s">
-        <v>38</v>
+        <v>267</v>
+      </c>
+      <c r="K42" t="b">
+        <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="43" spans="1:13">
       <c r="A43">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="K43" t="s">
         <v>38</v>
       </c>
       <c r="L43" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:13">
       <c r="A44">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="K44" t="s">
-        <v>271</v>
+        <v>38</v>
       </c>
       <c r="L44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:13">
       <c r="A45">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="K45" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="L45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="46" spans="1:13">
       <c r="A46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="K46" t="s">
-        <v>38</v>
+        <v>273</v>
       </c>
       <c r="L46" t="s">
-        <v>6</v>
-      </c>
-      <c r="M46" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47" spans="1:13">
       <c r="A47">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B47" t="s">
-        <v>275</v>
-      </c>
-      <c r="K47" t="b">
-        <v>1</v>
+        <v>274</v>
+      </c>
+      <c r="K47" t="s">
+        <v>38</v>
       </c>
       <c r="L47" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="M47" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:13">
       <c r="A48">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>276</v>
-      </c>
-      <c r="K48" t="s">
-        <v>38</v>
+        <v>275</v>
+      </c>
+      <c r="K48" t="b">
+        <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="A49">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>277</v>
-      </c>
-      <c r="K49" t="b">
-        <v>1</v>
+        <v>276</v>
+      </c>
+      <c r="K49" t="s">
+        <v>38</v>
+      </c>
+      <c r="L49" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:12">
@@ -7279,121 +7564,121 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="K50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="A51">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B51" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K51" t="b">
         <v>0</v>
       </c>
-      <c r="L51" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="52" spans="1:12">
       <c r="A52">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K52" t="b">
         <v>0</v>
       </c>
+      <c r="L52" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:12">
       <c r="A53">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>281</v>
-      </c>
-      <c r="K53" t="s">
-        <v>38</v>
-      </c>
-      <c r="L53" t="s">
-        <v>8</v>
+        <v>280</v>
+      </c>
+      <c r="K53" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="A54">
+        <v>7</v>
+      </c>
+      <c r="B54" t="s">
+        <v>281</v>
+      </c>
+      <c r="K54" t="s">
+        <v>38</v>
+      </c>
+      <c r="L54" t="s">
         <v>8</v>
-      </c>
-      <c r="B54" t="s">
-        <v>274</v>
-      </c>
-      <c r="K54" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="55" spans="1:12">
       <c r="A55">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B55" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="K55" t="s">
-        <v>283</v>
-      </c>
-      <c r="L55" t="s">
-        <v>1</v>
+        <v>38</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="A56">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B56" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="K56" t="s">
-        <v>38</v>
+        <v>283</v>
       </c>
       <c r="L56" t="s">
-        <v>285</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:12">
       <c r="A57">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B57" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="K57" t="s">
         <v>38</v>
       </c>
       <c r="L57" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="58" spans="1:12">
       <c r="A58">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="K58" t="s">
         <v>38</v>
+      </c>
+      <c r="L58" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="A59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B59" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K59" t="s">
         <v>38</v>
@@ -7404,130 +7689,130 @@
         <v>6</v>
       </c>
       <c r="B60" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K60" t="s">
-        <v>208</v>
+        <v>38</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="A61">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B61" t="s">
-        <v>291</v>
-      </c>
-      <c r="K61" t="b">
-        <v>1</v>
-      </c>
-      <c r="L61" t="s">
-        <v>9</v>
+        <v>290</v>
+      </c>
+      <c r="K61" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="A62">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>292</v>
-      </c>
-      <c r="K62" t="s">
-        <v>38</v>
+        <v>291</v>
+      </c>
+      <c r="K62" t="b">
+        <v>1</v>
       </c>
       <c r="L62" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="A63">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K63" t="s">
-        <v>294</v>
+        <v>38</v>
       </c>
       <c r="L63" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="A64">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="K64" t="s">
-        <v>38</v>
+        <v>294</v>
       </c>
       <c r="L64" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65" spans="1:13">
       <c r="A65">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>154</v>
+        <v>295</v>
       </c>
       <c r="K65" t="s">
         <v>38</v>
       </c>
       <c r="L65" t="s">
-        <v>296</v>
+        <v>11</v>
       </c>
     </row>
     <row r="66" spans="1:13">
       <c r="A66">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>297</v>
+        <v>154</v>
       </c>
       <c r="K66" t="s">
         <v>38</v>
       </c>
       <c r="L66" t="s">
-        <v>12</v>
+        <v>296</v>
       </c>
     </row>
     <row r="67" spans="1:13">
       <c r="A67">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B67" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="K67" t="s">
         <v>38</v>
       </c>
       <c r="L67" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68" spans="1:13">
       <c r="A68">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B68" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="K68" t="s">
         <v>38</v>
+      </c>
+      <c r="L68" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="69" spans="1:13">
       <c r="A69">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B69" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="K69" t="s">
-        <v>301</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:13">
@@ -7535,122 +7820,122 @@
         <v>4</v>
       </c>
       <c r="B70" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="K70" t="s">
-        <v>303</v>
-      </c>
-      <c r="L70" t="s">
-        <v>14</v>
-      </c>
-      <c r="M70" t="s">
-        <v>15</v>
+        <v>301</v>
       </c>
     </row>
     <row r="71" spans="1:13">
       <c r="A71">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="K71" t="s">
-        <v>38</v>
+        <v>303</v>
+      </c>
+      <c r="L71" t="s">
+        <v>14</v>
+      </c>
+      <c r="M71" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:13">
       <c r="A72">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B72" t="s">
-        <v>305</v>
-      </c>
-      <c r="K72" t="b">
-        <v>0</v>
-      </c>
-      <c r="L72" t="s">
-        <v>16</v>
+        <v>304</v>
+      </c>
+      <c r="K72" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="73" spans="1:13">
       <c r="A73">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B73" t="s">
-        <v>306</v>
-      </c>
-      <c r="K73" t="s">
-        <v>38</v>
+        <v>305</v>
+      </c>
+      <c r="K73" t="b">
+        <v>0</v>
       </c>
       <c r="L73" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="74" spans="1:13">
       <c r="A74">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B74" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="K74" t="s">
         <v>38</v>
       </c>
       <c r="L74" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="75" spans="1:13">
       <c r="A75">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B75" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="K75" t="s">
         <v>38</v>
       </c>
       <c r="L75" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="76" spans="1:13">
       <c r="A76">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B76" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="K76" t="s">
-        <v>294</v>
+        <v>38</v>
       </c>
       <c r="L76" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="77" spans="1:13">
       <c r="A77">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B77" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K77" t="s">
-        <v>38</v>
+        <v>294</v>
       </c>
       <c r="L77" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="78" spans="1:13">
       <c r="A78">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B78" t="s">
-        <v>311</v>
-      </c>
-      <c r="K78" t="b">
-        <v>1</v>
+        <v>310</v>
+      </c>
+      <c r="K78" t="s">
+        <v>38</v>
+      </c>
+      <c r="L78" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="79" spans="1:13">
@@ -7658,99 +7943,99 @@
         <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K79" t="b">
-        <v>0</v>
-      </c>
-      <c r="L79" t="s">
-        <v>32</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:13">
       <c r="A80">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>313</v>
-      </c>
-      <c r="K80" t="s">
-        <v>38</v>
+        <v>312</v>
+      </c>
+      <c r="K80" t="b">
+        <v>0</v>
+      </c>
+      <c r="L80" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:12">
       <c r="A81">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K81" t="s">
-        <v>273</v>
+        <v>38</v>
       </c>
     </row>
     <row r="82" spans="1:12">
       <c r="A82">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K82" t="s">
-        <v>38</v>
-      </c>
-      <c r="L82" t="s">
-        <v>19</v>
+        <v>273</v>
       </c>
     </row>
     <row r="83" spans="1:12">
       <c r="A83">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B83" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K83" t="s">
         <v>38</v>
       </c>
       <c r="L83" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="84" spans="1:12">
       <c r="A84">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="K84" t="s">
         <v>38</v>
+      </c>
+      <c r="L84" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="85" spans="1:12">
       <c r="A85">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>318</v>
-      </c>
-      <c r="K85" t="b">
-        <v>0</v>
-      </c>
-      <c r="L85" t="s">
-        <v>2</v>
+        <v>317</v>
+      </c>
+      <c r="K85" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="86" spans="1:12">
       <c r="A86">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B86" t="s">
-        <v>270</v>
-      </c>
-      <c r="K86" t="s">
-        <v>271</v>
+        <v>318</v>
+      </c>
+      <c r="K86" t="b">
+        <v>0</v>
+      </c>
+      <c r="L86" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="87" spans="1:12">
@@ -7758,10 +8043,10 @@
         <v>6</v>
       </c>
       <c r="B87" t="s">
-        <v>289</v>
+        <v>270</v>
       </c>
       <c r="K87" t="s">
-        <v>38</v>
+        <v>271</v>
       </c>
     </row>
     <row r="88" spans="1:12">
@@ -7769,35 +8054,35 @@
         <v>6</v>
       </c>
       <c r="B88" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="K88" t="s">
-        <v>208</v>
+        <v>38</v>
       </c>
     </row>
     <row r="89" spans="1:12">
       <c r="A89">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B89" t="s">
-        <v>319</v>
+        <v>290</v>
       </c>
       <c r="K89" t="s">
-        <v>301</v>
-      </c>
-      <c r="L89" t="s">
-        <v>7</v>
+        <v>208</v>
       </c>
     </row>
     <row r="90" spans="1:12">
       <c r="A90">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B90" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="K90" t="s">
-        <v>38</v>
+        <v>301</v>
+      </c>
+      <c r="L90" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="91" spans="1:12">
@@ -7805,88 +8090,88 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>318</v>
-      </c>
-      <c r="K91" t="b">
-        <v>0</v>
+        <v>307</v>
+      </c>
+      <c r="K91" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="92" spans="1:12">
       <c r="A92">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B92" t="s">
-        <v>302</v>
-      </c>
-      <c r="K92" t="s">
-        <v>303</v>
+        <v>318</v>
+      </c>
+      <c r="K92" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="A93">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B93" t="s">
-        <v>320</v>
+        <v>302</v>
       </c>
       <c r="K93" t="s">
-        <v>273</v>
-      </c>
-      <c r="L93" t="s">
-        <v>5</v>
+        <v>303</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="A94">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="K94" t="s">
-        <v>38</v>
+        <v>273</v>
       </c>
       <c r="L94" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="A95">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B95" t="s">
-        <v>322</v>
-      </c>
-      <c r="K95" t="b">
-        <v>1</v>
+        <v>321</v>
+      </c>
+      <c r="K95" t="s">
+        <v>38</v>
       </c>
       <c r="L95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="A96">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B96" t="s">
-        <v>323</v>
-      </c>
-      <c r="K96" t="s">
-        <v>38</v>
+        <v>322</v>
+      </c>
+      <c r="K96" t="b">
+        <v>1</v>
       </c>
       <c r="L96" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="97" spans="1:13">
       <c r="A97">
+        <v>6</v>
+      </c>
+      <c r="B97" t="s">
+        <v>323</v>
+      </c>
+      <c r="K97" t="s">
+        <v>38</v>
+      </c>
+      <c r="L97" t="s">
         <v>7</v>
-      </c>
-      <c r="B97" t="s">
-        <v>324</v>
-      </c>
-      <c r="K97" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="98" spans="1:13">
@@ -7894,32 +8179,32 @@
         <v>7</v>
       </c>
       <c r="B98" t="s">
-        <v>325</v>
-      </c>
-      <c r="K98" t="b">
-        <v>1</v>
+        <v>324</v>
+      </c>
+      <c r="K98" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="99" spans="1:13">
       <c r="A99">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B99" t="s">
-        <v>326</v>
-      </c>
-      <c r="K99" t="s">
-        <v>303</v>
+        <v>325</v>
+      </c>
+      <c r="K99" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:13">
       <c r="A100">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B100" t="s">
-        <v>327</v>
-      </c>
-      <c r="K100" t="b">
-        <v>0</v>
+        <v>326</v>
+      </c>
+      <c r="K100" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="101" spans="1:13">
@@ -7927,41 +8212,41 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>328</v>
-      </c>
-      <c r="K101" t="s">
-        <v>273</v>
-      </c>
-      <c r="L101" t="s">
-        <v>23</v>
+        <v>327</v>
+      </c>
+      <c r="K101" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:13">
       <c r="A102">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B102" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="K102" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="L102" t="s">
-        <v>330</v>
-      </c>
-      <c r="M102" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="103" spans="1:13">
       <c r="A103">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B103" t="s">
-        <v>331</v>
-      </c>
-      <c r="K103" t="b">
-        <v>1</v>
+        <v>329</v>
+      </c>
+      <c r="K103" t="s">
+        <v>283</v>
+      </c>
+      <c r="L103" t="s">
+        <v>330</v>
+      </c>
+      <c r="M103" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="104" spans="1:13">
@@ -7969,38 +8254,38 @@
         <v>7</v>
       </c>
       <c r="B104" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K104" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:13">
       <c r="A105">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B105" t="s">
-        <v>333</v>
-      </c>
-      <c r="K105" t="s">
-        <v>38</v>
-      </c>
-      <c r="L105" t="s">
-        <v>24</v>
-      </c>
-      <c r="M105" t="s">
-        <v>25</v>
+        <v>332</v>
+      </c>
+      <c r="K105" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:13">
       <c r="A106">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B106" t="s">
-        <v>331</v>
-      </c>
-      <c r="K106" t="b">
-        <v>1</v>
+        <v>333</v>
+      </c>
+      <c r="K106" t="s">
+        <v>38</v>
+      </c>
+      <c r="L106" t="s">
+        <v>24</v>
+      </c>
+      <c r="M106" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="107" spans="1:13">
@@ -8008,80 +8293,77 @@
         <v>7</v>
       </c>
       <c r="B107" t="s">
+        <v>331</v>
+      </c>
+      <c r="K107" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13">
+      <c r="A108">
+        <v>7</v>
+      </c>
+      <c r="B108" t="s">
         <v>332</v>
       </c>
-      <c r="K107" t="b">
+      <c r="K108" t="b">
         <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13">
-      <c r="A109">
-        <v>0</v>
-      </c>
-      <c r="B109" t="s">
-        <v>337</v>
-      </c>
-      <c r="L109" t="s">
-        <v>334</v>
-      </c>
-      <c r="M109" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="110" spans="1:13">
       <c r="A110">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B110" t="s">
-        <v>347</v>
-      </c>
-      <c r="K110" t="s">
-        <v>38</v>
+        <v>337</v>
       </c>
       <c r="L110" t="s">
-        <v>339</v>
+        <v>334</v>
+      </c>
+      <c r="M110" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="111" spans="1:13">
       <c r="A111">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B111" t="s">
-        <v>352</v>
+        <v>346</v>
       </c>
       <c r="K111" t="s">
         <v>38</v>
       </c>
       <c r="L111" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="112" spans="1:13">
       <c r="A112">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>348</v>
+        <v>374</v>
       </c>
       <c r="K112" t="s">
-        <v>341</v>
+        <v>38</v>
       </c>
       <c r="L112" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="113" spans="1:13">
       <c r="A113">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="K113" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="L113" t="s">
-        <v>345</v>
+        <v>358</v>
       </c>
     </row>
     <row r="114" spans="1:13">
@@ -8089,24 +8371,24 @@
         <v>4</v>
       </c>
       <c r="B114" t="s">
-        <v>353</v>
-      </c>
-      <c r="K114" t="s">
+        <v>348</v>
+      </c>
+      <c r="K114" t="b">
+        <v>0</v>
+      </c>
+      <c r="L114" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="115" spans="1:13">
       <c r="A115">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B115" t="s">
-        <v>350</v>
+        <v>375</v>
       </c>
       <c r="K115" t="s">
-        <v>342</v>
-      </c>
-      <c r="L115" t="s">
-        <v>346</v>
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="1:13">
@@ -8114,108 +8396,108 @@
         <v>4</v>
       </c>
       <c r="B116" t="s">
-        <v>355</v>
-      </c>
-      <c r="K116" t="s">
-        <v>38</v>
-      </c>
-      <c r="L116" t="s">
-        <v>354</v>
+        <v>351</v>
+      </c>
+      <c r="K116" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:13">
       <c r="A117">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>359</v>
+        <v>349</v>
       </c>
       <c r="K117" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L117" t="s">
-        <v>357</v>
-      </c>
-      <c r="M117" t="s">
-        <v>358</v>
+        <v>345</v>
       </c>
     </row>
     <row r="118" spans="1:13">
       <c r="A118">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B118" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="K118" t="s">
         <v>38</v>
       </c>
       <c r="L118" t="s">
-        <v>21</v>
+        <v>352</v>
       </c>
     </row>
     <row r="119" spans="1:13">
       <c r="A119">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B119" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="K119" t="s">
-        <v>341</v>
+        <v>283</v>
       </c>
       <c r="L119" t="s">
-        <v>364</v>
+        <v>372</v>
       </c>
     </row>
     <row r="120" spans="1:13">
       <c r="A120">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B120" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="K120" t="s">
-        <v>343</v>
+        <v>341</v>
+      </c>
+      <c r="L120" t="s">
+        <v>371</v>
+      </c>
+      <c r="M120" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="121" spans="1:13">
       <c r="A121">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B121" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="K121" t="s">
-        <v>344</v>
+        <v>38</v>
+      </c>
+      <c r="L121" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="122" spans="1:13">
       <c r="A122">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B122" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="K122" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="L122" t="s">
-        <v>364</v>
+        <v>355</v>
       </c>
     </row>
     <row r="123" spans="1:13">
       <c r="A123">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B123" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="K123" t="s">
-        <v>28</v>
-      </c>
-      <c r="L123" t="s">
-        <v>370</v>
+        <v>342</v>
       </c>
     </row>
     <row r="124" spans="1:13">
@@ -8223,10 +8505,10 @@
         <v>9</v>
       </c>
       <c r="B124" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="K124" t="s">
-        <v>38</v>
+        <v>343</v>
       </c>
     </row>
     <row r="125" spans="1:13">
@@ -8234,13 +8516,13 @@
         <v>8</v>
       </c>
       <c r="B125" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="K125" t="s">
-        <v>29</v>
+        <v>341</v>
       </c>
       <c r="L125" t="s">
-        <v>369</v>
+        <v>355</v>
       </c>
     </row>
     <row r="126" spans="1:13">
@@ -8248,72 +8530,141 @@
         <v>9</v>
       </c>
       <c r="B126" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="K126" t="s">
-        <v>38</v>
+        <v>28</v>
+      </c>
+      <c r="L126" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="127" spans="1:13">
       <c r="A127">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B127" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="K127" t="s">
-        <v>341</v>
-      </c>
-      <c r="L127" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
     </row>
     <row r="128" spans="1:13">
       <c r="A128">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B128" t="s">
-        <v>360</v>
+        <v>368</v>
       </c>
       <c r="K128" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="L128" t="s">
-        <v>21</v>
+        <v>356</v>
       </c>
     </row>
     <row r="129" spans="1:13">
       <c r="A129">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B129" t="s">
-        <v>351</v>
-      </c>
-      <c r="K129" t="b">
-        <v>1</v>
-      </c>
-      <c r="L129" t="s">
-        <v>335</v>
-      </c>
-      <c r="M129" t="s">
-        <v>41</v>
+        <v>359</v>
+      </c>
+      <c r="K129" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="130" spans="1:13">
       <c r="A130">
+        <v>6</v>
+      </c>
+      <c r="B130" t="s">
+        <v>370</v>
+      </c>
+      <c r="K130" t="s">
+        <v>340</v>
+      </c>
+      <c r="L130" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="131" spans="1:13">
+      <c r="A131">
+        <v>7</v>
+      </c>
+      <c r="B131" t="s">
+        <v>364</v>
+      </c>
+      <c r="K131" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13">
+      <c r="A132">
+        <v>5</v>
+      </c>
+      <c r="B132" t="s">
+        <v>369</v>
+      </c>
+      <c r="K132" t="s">
+        <v>38</v>
+      </c>
+      <c r="L132" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13">
+      <c r="A133">
+        <v>6</v>
+      </c>
+      <c r="B133" t="s">
+        <v>363</v>
+      </c>
+      <c r="K133" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13">
+      <c r="A134">
+        <v>6</v>
+      </c>
+      <c r="B134" t="s">
+        <v>370</v>
+      </c>
+      <c r="K134" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="135" spans="1:13">
+      <c r="A135">
+        <v>1</v>
+      </c>
+      <c r="B135" t="s">
+        <v>350</v>
+      </c>
+      <c r="K135" t="b">
+        <v>1</v>
+      </c>
+      <c r="L135" t="s">
+        <v>335</v>
+      </c>
+      <c r="M135" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="136" spans="1:13">
+      <c r="A136">
         <v>2</v>
       </c>
-      <c r="B130" t="s">
+      <c r="B136" t="s">
         <v>336</v>
       </c>
-      <c r="K130" t="s">
-        <v>38</v>
-      </c>
-      <c r="L130" t="s">
-        <v>371</v>
-      </c>
-      <c r="M130" t="s">
-        <v>372</v>
+      <c r="K136" t="s">
+        <v>38</v>
+      </c>
+      <c r="L136" t="s">
+        <v>376</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Prediction Phase In Progress
- Change RecordNo to be an int
- Remove reference of “Applicant” in server side code
- Add Prediction record UI
- Fix bug for target factor carried over from Phase 2 to Phase 3
</commit_message>
<xml_diff>
--- a/auto-agent/workflow.xlsx
+++ b/auto-agent/workflow.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="20" yWindow="0" windowWidth="25360" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="workflowText.csv" sheetId="19" r:id="rId1"/>
+    <sheet name="workflowText.csv" sheetId="21" r:id="rId1"/>
     <sheet name="template" sheetId="5" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="423">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="426">
   <si>
     <t>So, what do you think? Overall do you think {{.TargetFactor.FactorName}} makes a difference to performance in space?</t>
   </si>
@@ -55,9 +55,6 @@
     <t>I see. Now, how do you think the chart would look different if {{.TargetFactor.FactorName}} makes no difference to performance?</t>
   </si>
   <si>
-    <t>Great! Thank you for the memo to the foundation. Let's move on to the next factor then.</t>
-  </si>
-  <si>
     <t>I see. Let's look at the performance of all of the people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$alevel := index $factor.Levels 1}}{{$alevel.Text}} for {{.TargetFactor.FactorName}}. What is the best performance those people have?</t>
   </si>
   <si>
@@ -1177,9 +1174,6 @@
     <t xml:space="preserve">        all_correct_causal.2</t>
   </si>
   <si>
-    <t>Now, look at the applicant on the screen. What do you think the applicant's performance will be?</t>
-  </si>
-  <si>
     <t>start_prediction</t>
   </si>
   <si>
@@ -1189,12 +1183,6 @@
     <t>Great. Now you are ready to make some predictions. Press "Enter" to continue.</t>
   </si>
   <si>
-    <t>Let's take a look at an applicant.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
     <t>Now, I have some new applicants here. You can use what you found to predict how well they will do and pick a best team of five!</t>
   </si>
   <si>
@@ -1204,9 +1192,6 @@
     <t>I can only tell you up to four things about the applicant. Which factors do you want to know about? Pick all of the ones you need so you can predict their performance.</t>
   </si>
   <si>
-    <t>Here are the information about {{range $i, $v := .DisplayFactors}}{{if eq $i 3}} and {{else if gt $i 0}}, {{end}}{{$v.Text}}{{end}} for {{.TargetApplicant.Name}}.</t>
-  </si>
-  <si>
     <t xml:space="preserve">            wrong.show_chart.MC_is_needed.1</t>
   </si>
   <si>
@@ -1288,7 +1273,31 @@
     <t xml:space="preserve">                         wrong.wrong.causal.1.2.2</t>
   </si>
   <si>
-    <t>Ok, so you want to know about {{$length := len .RequestedFactors}}{{range $i, $v := .RequestedFactors}}{{if eq $i 2}}{{if eq $length 3}} and {{else}}, {{end}}{{else if eq $i 3}} and {{else if gt $i 0}}, {{end}}{{$v.Text}}{{end}}.</t>
+    <t>Alright, you want to know about {{$length := len .RequestedFactors}}{{range $i, $v := .RequestedFactors}}{{if eq $i 2}}{{if eq $length 3}} and {{else}}, {{end}}{{else if eq $i 3}} and {{else if gt $i 0}}, {{end}}{{$v.Text}}{{end}}.</t>
+  </si>
+  <si>
+    <t>Great! Thank you for the memo to the foundation. Let's move on to the next thing then.</t>
+  </si>
+  <si>
+    <t>Let's take a look at Applicant #{{.TargetPrediction.RecordNo}},  {{.TargetPrediction.RecordName}}</t>
+  </si>
+  <si>
+    <t>Here are the information about {{range $i, $v := .DisplayFactors}}{{if eq $i 3}} and {{else if gt $i 0}}, {{end}}{{$v.Text}}{{end}} for {{.TargetPrediction.RecordName}}. What do you think {{.TargetPrediction.FirstName}}'s performance will be?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        correct_perf.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        incorrect_perf.1</t>
+  </si>
+  <si>
+    <t>Ok, you think {{.TargetPrediction.FirstName}} will have {{.TargetPrediction.PredictedPerformanceLevel}}.</t>
+  </si>
+  <si>
+    <t>Ok, you think {{.TargetPrediction.FirstName}} will have {{.TargetPrediction.PredictedPerformanceLevel}}. Which of the four factors you have data on mattered to your prediction?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
   </si>
 </sst>
 </file>
@@ -1337,8 +1346,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1699">
+  <cellStyleXfs count="1719">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3041,7 +3070,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1699">
+  <cellStyles count="1719">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -3891,6 +3920,16 @@
     <cellStyle name="Followed Hyperlink" xfId="1694" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1696" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1698" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1700" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1702" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1704" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1706" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1708" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1710" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1712" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1714" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1716" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1718" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -4740,6 +4779,16 @@
     <cellStyle name="Hyperlink" xfId="1693" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1695" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1697" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1699" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1701" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1703" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1705" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1707" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1709" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1711" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1713" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1715" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1717" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -5069,18 +5118,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F258"/>
+  <dimension ref="A1:F261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <cols>
-    <col min="2" max="2" width="64.1640625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -5088,13 +5134,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" t="s">
         <v>24</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
       <c r="E2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -5102,10 +5148,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -5113,16 +5159,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" t="b">
         <v>1</v>
       </c>
       <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
         <v>29</v>
-      </c>
-      <c r="E4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -5130,16 +5176,16 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>359</v>
+      </c>
+      <c r="E5" t="s">
         <v>31</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>360</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -5147,16 +5193,16 @@
         <v>0</v>
       </c>
       <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>35</v>
-      </c>
-      <c r="F6" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -5164,16 +5210,16 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
-      </c>
-      <c r="E7" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -5181,10 +5227,10 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" t="s">
         <v>40</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -5192,16 +5238,16 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -5209,16 +5255,16 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" t="s">
         <v>45</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>46</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -5226,13 +5272,13 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -5240,13 +5286,13 @@
         <v>4</v>
       </c>
       <c r="B12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
         <v>50</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -5254,13 +5300,13 @@
         <v>5</v>
       </c>
       <c r="B13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>52</v>
-      </c>
-      <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -5268,13 +5314,13 @@
         <v>6</v>
       </c>
       <c r="B14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" t="s">
         <v>54</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>55</v>
-      </c>
-      <c r="D14" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -5282,13 +5328,13 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
+        <v>56</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D15" t="s">
         <v>57</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -5296,13 +5342,13 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
         <v>59</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -5310,13 +5356,13 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
         <v>62</v>
-      </c>
-      <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -5324,13 +5370,13 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" t="s">
         <v>64</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -5338,16 +5384,16 @@
         <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" t="s">
         <v>66</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>67</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>68</v>
-      </c>
-      <c r="E19" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -5355,10 +5401,10 @@
         <v>12</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -5366,13 +5412,13 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D21" t="s">
         <v>71</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -5380,10 +5426,10 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -5391,10 +5437,10 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -5402,10 +5448,10 @@
         <v>8</v>
       </c>
       <c r="B24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -5413,16 +5459,16 @@
         <v>6</v>
       </c>
       <c r="B25" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" t="s">
         <v>76</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
         <v>77</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>78</v>
-      </c>
-      <c r="E25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -5430,10 +5476,10 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -5441,16 +5487,16 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" t="s">
         <v>81</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>82</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>83</v>
-      </c>
-      <c r="E27" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -5458,16 +5504,16 @@
         <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" t="s">
+        <v>66</v>
+      </c>
+      <c r="D28" t="s">
         <v>67</v>
       </c>
-      <c r="D28" t="s">
-        <v>68</v>
-      </c>
       <c r="E28" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -5475,10 +5521,10 @@
         <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -5486,13 +5532,13 @@
         <v>3</v>
       </c>
       <c r="B30" t="s">
+        <v>85</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
         <v>86</v>
-      </c>
-      <c r="C30" t="s">
-        <v>27</v>
-      </c>
-      <c r="D30" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -5500,13 +5546,13 @@
         <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" t="s">
         <v>88</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -5514,13 +5560,13 @@
         <v>5</v>
       </c>
       <c r="B32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="D32" t="s">
         <v>90</v>
-      </c>
-      <c r="C32" t="s">
-        <v>27</v>
-      </c>
-      <c r="D32" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -5528,13 +5574,13 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C33" t="b">
         <v>1</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -5542,13 +5588,13 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
         <v>94</v>
       </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>95</v>
-      </c>
-      <c r="D34" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -5556,10 +5602,10 @@
         <v>8</v>
       </c>
       <c r="B35" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -5567,13 +5613,13 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
         <v>98</v>
       </c>
-      <c r="C36" t="s">
-        <v>99</v>
-      </c>
       <c r="D36" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -5581,13 +5627,13 @@
         <v>8</v>
       </c>
       <c r="B37" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s">
+        <v>54</v>
+      </c>
+      <c r="D37" t="s">
         <v>100</v>
-      </c>
-      <c r="C37" t="s">
-        <v>55</v>
-      </c>
-      <c r="D37" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -5595,10 +5641,10 @@
         <v>9</v>
       </c>
       <c r="B38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C38" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -5606,16 +5652,16 @@
         <v>8</v>
       </c>
       <c r="B39" t="s">
+        <v>102</v>
+      </c>
+      <c r="C39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" t="s">
         <v>103</v>
       </c>
-      <c r="C39" t="s">
-        <v>77</v>
-      </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>104</v>
-      </c>
-      <c r="E39" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -5623,10 +5669,10 @@
         <v>9</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -5634,13 +5680,13 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41" t="s">
         <v>107</v>
       </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>108</v>
-      </c>
-      <c r="D41" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -5648,13 +5694,13 @@
         <v>8</v>
       </c>
       <c r="B42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" t="s">
+        <v>26</v>
+      </c>
+      <c r="D42" t="s">
         <v>110</v>
-      </c>
-      <c r="C42" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -5662,10 +5708,10 @@
         <v>9</v>
       </c>
       <c r="B43" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C43" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -5673,13 +5719,13 @@
         <v>8</v>
       </c>
       <c r="B44" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C44" t="b">
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -5687,13 +5733,13 @@
         <v>9</v>
       </c>
       <c r="B45" t="s">
+        <v>114</v>
+      </c>
+      <c r="C45" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" t="s">
         <v>115</v>
-      </c>
-      <c r="C45" t="s">
-        <v>27</v>
-      </c>
-      <c r="D45" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -5701,13 +5747,13 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" t="s">
         <v>117</v>
-      </c>
-      <c r="C46" t="s">
-        <v>55</v>
-      </c>
-      <c r="D46" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -5715,16 +5761,16 @@
         <v>11</v>
       </c>
       <c r="B47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C47" t="s">
+        <v>26</v>
+      </c>
+      <c r="D47" t="s">
         <v>119</v>
       </c>
-      <c r="C47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>120</v>
-      </c>
-      <c r="E47" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -5732,13 +5778,13 @@
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C48" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D48" t="s">
-        <v>11</v>
+        <v>418</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -5746,13 +5792,13 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
+        <v>122</v>
+      </c>
+      <c r="C49" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" t="s">
         <v>123</v>
-      </c>
-      <c r="C49" t="s">
-        <v>77</v>
-      </c>
-      <c r="D49" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -5760,13 +5806,13 @@
         <v>11</v>
       </c>
       <c r="B50" t="s">
+        <v>124</v>
+      </c>
+      <c r="C50" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" t="s">
         <v>125</v>
-      </c>
-      <c r="C50" t="s">
-        <v>27</v>
-      </c>
-      <c r="D50" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -5774,10 +5820,10 @@
         <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C51" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -5785,13 +5831,13 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" t="b">
         <v>0</v>
       </c>
       <c r="D52" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -5799,13 +5845,13 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
+        <v>129</v>
+      </c>
+      <c r="C53" t="s">
+        <v>94</v>
+      </c>
+      <c r="D53" t="s">
         <v>130</v>
-      </c>
-      <c r="C53" t="s">
-        <v>95</v>
-      </c>
-      <c r="D53" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -5813,10 +5859,10 @@
         <v>8</v>
       </c>
       <c r="B54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C54" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -5824,13 +5870,13 @@
         <v>7</v>
       </c>
       <c r="B55" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D55" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -5838,10 +5884,10 @@
         <v>8</v>
       </c>
       <c r="B56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C56" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -5849,13 +5895,13 @@
         <v>7</v>
       </c>
       <c r="B57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C57" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D57" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -5863,13 +5909,13 @@
         <v>8</v>
       </c>
       <c r="B58" t="s">
+        <v>135</v>
+      </c>
+      <c r="C58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D58" t="s">
         <v>136</v>
-      </c>
-      <c r="C58" t="s">
-        <v>27</v>
-      </c>
-      <c r="D58" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -5877,10 +5923,10 @@
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C59" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -5888,13 +5934,13 @@
         <v>8</v>
       </c>
       <c r="B60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C60" t="b">
         <v>0</v>
       </c>
       <c r="D60" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -5902,10 +5948,10 @@
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -5913,13 +5959,13 @@
         <v>6</v>
       </c>
       <c r="B62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C62" t="s">
+        <v>26</v>
+      </c>
+      <c r="D62" t="s">
         <v>141</v>
-      </c>
-      <c r="C62" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -5927,16 +5973,16 @@
         <v>7</v>
       </c>
       <c r="B63" t="s">
+        <v>142</v>
+      </c>
+      <c r="C63" t="s">
+        <v>94</v>
+      </c>
+      <c r="D63" t="s">
         <v>143</v>
       </c>
-      <c r="C63" t="s">
-        <v>95</v>
-      </c>
-      <c r="D63" t="s">
-        <v>144</v>
-      </c>
       <c r="E63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -5944,10 +5990,10 @@
         <v>8</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -5955,16 +6001,16 @@
         <v>7</v>
       </c>
       <c r="B65" t="s">
+        <v>144</v>
+      </c>
+      <c r="C65" t="s">
+        <v>26</v>
+      </c>
+      <c r="D65" t="s">
         <v>145</v>
       </c>
-      <c r="C65" t="s">
-        <v>27</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="E65" t="s">
         <v>146</v>
-      </c>
-      <c r="E65" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -5972,16 +6018,16 @@
         <v>8</v>
       </c>
       <c r="B66" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C66" t="b">
         <v>1</v>
       </c>
       <c r="D66" t="s">
+        <v>148</v>
+      </c>
+      <c r="E66" t="s">
         <v>149</v>
-      </c>
-      <c r="E66" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -5989,13 +6035,13 @@
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C67" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -6003,16 +6049,16 @@
         <v>10</v>
       </c>
       <c r="B68" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C68" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D68" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E68" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -6020,13 +6066,13 @@
         <v>11</v>
       </c>
       <c r="B69" t="s">
+        <v>152</v>
+      </c>
+      <c r="C69" t="s">
+        <v>26</v>
+      </c>
+      <c r="D69" t="s">
         <v>153</v>
-      </c>
-      <c r="C69" t="s">
-        <v>27</v>
-      </c>
-      <c r="D69" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -6034,10 +6080,10 @@
         <v>12</v>
       </c>
       <c r="B70" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C70" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -6045,10 +6091,10 @@
         <v>12</v>
       </c>
       <c r="B71" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C71" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -6056,13 +6102,13 @@
         <v>9</v>
       </c>
       <c r="B72" t="s">
+        <v>156</v>
+      </c>
+      <c r="C72" t="s">
+        <v>107</v>
+      </c>
+      <c r="D72" t="s">
         <v>157</v>
-      </c>
-      <c r="C72" t="s">
-        <v>108</v>
-      </c>
-      <c r="D72" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -6070,10 +6116,10 @@
         <v>10</v>
       </c>
       <c r="B73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C73" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -6081,13 +6127,13 @@
         <v>10</v>
       </c>
       <c r="B74" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C74" t="b">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -6095,10 +6141,10 @@
         <v>11</v>
       </c>
       <c r="B75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C75" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -6106,16 +6152,16 @@
         <v>8</v>
       </c>
       <c r="B76" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C76" t="b">
         <v>0</v>
       </c>
       <c r="D76" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -6123,13 +6169,13 @@
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C77" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D77" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -6137,19 +6183,19 @@
         <v>10</v>
       </c>
       <c r="B78" t="s">
+        <v>165</v>
+      </c>
+      <c r="C78" t="s">
+        <v>26</v>
+      </c>
+      <c r="D78" t="s">
+        <v>132</v>
+      </c>
+      <c r="E78" t="s">
         <v>166</v>
       </c>
-      <c r="C78" t="s">
-        <v>27</v>
-      </c>
-      <c r="D78" t="s">
-        <v>133</v>
-      </c>
-      <c r="E78" t="s">
-        <v>167</v>
-      </c>
       <c r="F78" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -6157,10 +6203,10 @@
         <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C79" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -6168,13 +6214,13 @@
         <v>9</v>
       </c>
       <c r="B80" t="s">
+        <v>167</v>
+      </c>
+      <c r="C80" t="s">
+        <v>107</v>
+      </c>
+      <c r="D80" t="s">
         <v>168</v>
-      </c>
-      <c r="C80" t="s">
-        <v>108</v>
-      </c>
-      <c r="D80" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -6182,10 +6228,10 @@
         <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C81" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -6193,13 +6239,13 @@
         <v>10</v>
       </c>
       <c r="B82" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C82" t="b">
         <v>0</v>
       </c>
       <c r="D82" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -6207,10 +6253,10 @@
         <v>11</v>
       </c>
       <c r="B83" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C83" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -6218,16 +6264,16 @@
         <v>8</v>
       </c>
       <c r="B84" t="s">
+        <v>171</v>
+      </c>
+      <c r="C84" t="s">
+        <v>26</v>
+      </c>
+      <c r="D84" t="s">
         <v>172</v>
       </c>
-      <c r="C84" t="s">
-        <v>27</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>173</v>
-      </c>
-      <c r="E84" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -6235,13 +6281,13 @@
         <v>9</v>
       </c>
       <c r="B85" t="s">
+        <v>174</v>
+      </c>
+      <c r="C85" t="s">
+        <v>26</v>
+      </c>
+      <c r="D85" t="s">
         <v>175</v>
-      </c>
-      <c r="C85" t="s">
-        <v>27</v>
-      </c>
-      <c r="D85" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -6249,15 +6295,15 @@
         <v>10</v>
       </c>
       <c r="B86" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C86" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -6265,13 +6311,13 @@
         <v>0</v>
       </c>
       <c r="B88" t="s">
+        <v>178</v>
+      </c>
+      <c r="D88" t="s">
         <v>179</v>
       </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>180</v>
-      </c>
-      <c r="E88" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -6279,16 +6325,16 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
+        <v>181</v>
+      </c>
+      <c r="C89" t="s">
+        <v>26</v>
+      </c>
+      <c r="D89" t="s">
         <v>182</v>
       </c>
-      <c r="C89" t="s">
-        <v>27</v>
-      </c>
-      <c r="D89" t="s">
-        <v>183</v>
-      </c>
       <c r="E89" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -6296,13 +6342,13 @@
         <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D90" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -6310,13 +6356,13 @@
         <v>3</v>
       </c>
       <c r="B91" t="s">
+        <v>184</v>
+      </c>
+      <c r="C91" t="s">
+        <v>26</v>
+      </c>
+      <c r="D91" t="s">
         <v>185</v>
-      </c>
-      <c r="C91" t="s">
-        <v>27</v>
-      </c>
-      <c r="D91" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -6324,10 +6370,10 @@
         <v>4</v>
       </c>
       <c r="B92" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C92" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -6335,13 +6381,13 @@
         <v>3</v>
       </c>
       <c r="B93" t="s">
+        <v>187</v>
+      </c>
+      <c r="C93" t="s">
         <v>188</v>
       </c>
-      <c r="C93" t="s">
+      <c r="D93" t="s">
         <v>189</v>
-      </c>
-      <c r="D93" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -6349,10 +6395,10 @@
         <v>4</v>
       </c>
       <c r="B94" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C94" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -6360,13 +6406,13 @@
         <v>3</v>
       </c>
       <c r="B95" t="s">
+        <v>191</v>
+      </c>
+      <c r="C95" t="s">
         <v>192</v>
       </c>
-      <c r="C95" t="s">
+      <c r="D95" t="s">
         <v>193</v>
-      </c>
-      <c r="D95" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -6374,13 +6420,13 @@
         <v>4</v>
       </c>
       <c r="B96" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C96" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D96" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -6388,13 +6434,13 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
+        <v>194</v>
+      </c>
+      <c r="C97" t="s">
+        <v>26</v>
+      </c>
+      <c r="D97" t="s">
         <v>195</v>
-      </c>
-      <c r="C97" t="s">
-        <v>27</v>
-      </c>
-      <c r="D97" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -6402,13 +6448,13 @@
         <v>6</v>
       </c>
       <c r="B98" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C98" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D98" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -6416,13 +6462,13 @@
         <v>7</v>
       </c>
       <c r="B99" t="s">
+        <v>197</v>
+      </c>
+      <c r="C99" t="s">
+        <v>26</v>
+      </c>
+      <c r="D99" t="s">
         <v>198</v>
-      </c>
-      <c r="C99" t="s">
-        <v>27</v>
-      </c>
-      <c r="D99" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -6430,10 +6476,10 @@
         <v>8</v>
       </c>
       <c r="B100" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -6441,10 +6487,10 @@
         <v>7</v>
       </c>
       <c r="B101" t="s">
+        <v>200</v>
+      </c>
+      <c r="C101" t="s">
         <v>201</v>
-      </c>
-      <c r="C101" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -6452,10 +6498,10 @@
         <v>6</v>
       </c>
       <c r="B102" t="s">
+        <v>202</v>
+      </c>
+      <c r="C102" t="s">
         <v>203</v>
-      </c>
-      <c r="C102" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -6463,13 +6509,13 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
+        <v>204</v>
+      </c>
+      <c r="C103" t="s">
         <v>205</v>
       </c>
-      <c r="C103" t="s">
-        <v>206</v>
-      </c>
       <c r="D103" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -6477,13 +6523,13 @@
         <v>6</v>
       </c>
       <c r="B104" t="s">
+        <v>206</v>
+      </c>
+      <c r="C104" t="s">
+        <v>26</v>
+      </c>
+      <c r="D104" t="s">
         <v>207</v>
-      </c>
-      <c r="C104" t="s">
-        <v>27</v>
-      </c>
-      <c r="D104" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -6491,13 +6537,13 @@
         <v>7</v>
       </c>
       <c r="B105" t="s">
+        <v>208</v>
+      </c>
+      <c r="C105" t="s">
+        <v>26</v>
+      </c>
+      <c r="D105" t="s">
         <v>209</v>
-      </c>
-      <c r="C105" t="s">
-        <v>27</v>
-      </c>
-      <c r="D105" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -6505,10 +6551,10 @@
         <v>8</v>
       </c>
       <c r="B106" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C106" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -6516,10 +6562,10 @@
         <v>8</v>
       </c>
       <c r="B107" t="s">
+        <v>211</v>
+      </c>
+      <c r="C107" t="s">
         <v>212</v>
-      </c>
-      <c r="C107" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -6527,13 +6573,13 @@
         <v>6</v>
       </c>
       <c r="B108" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D108" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -6541,13 +6587,13 @@
         <v>7</v>
       </c>
       <c r="B109" t="s">
+        <v>214</v>
+      </c>
+      <c r="C109" t="s">
+        <v>26</v>
+      </c>
+      <c r="D109" t="s">
         <v>215</v>
-      </c>
-      <c r="C109" t="s">
-        <v>27</v>
-      </c>
-      <c r="D109" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -6555,10 +6601,10 @@
         <v>8</v>
       </c>
       <c r="B110" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C110" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -6566,13 +6612,13 @@
         <v>7</v>
       </c>
       <c r="B111" t="s">
+        <v>217</v>
+      </c>
+      <c r="C111" t="s">
         <v>218</v>
       </c>
-      <c r="C111" t="s">
-        <v>219</v>
-      </c>
       <c r="D111" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -6580,16 +6626,16 @@
         <v>8</v>
       </c>
       <c r="B112" t="s">
+        <v>219</v>
+      </c>
+      <c r="C112" t="s">
+        <v>26</v>
+      </c>
+      <c r="D112" t="s">
         <v>220</v>
       </c>
-      <c r="C112" t="s">
-        <v>27</v>
-      </c>
-      <c r="D112" t="s">
+      <c r="E112" t="s">
         <v>221</v>
-      </c>
-      <c r="E112" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -6597,13 +6643,13 @@
         <v>9</v>
       </c>
       <c r="B113" t="s">
+        <v>222</v>
+      </c>
+      <c r="C113" t="s">
+        <v>26</v>
+      </c>
+      <c r="D113" t="s">
         <v>223</v>
-      </c>
-      <c r="C113" t="s">
-        <v>27</v>
-      </c>
-      <c r="D113" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -6611,10 +6657,10 @@
         <v>10</v>
       </c>
       <c r="B114" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C114" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -6622,13 +6668,13 @@
         <v>9</v>
       </c>
       <c r="B115" t="s">
+        <v>225</v>
+      </c>
+      <c r="C115" t="s">
+        <v>218</v>
+      </c>
+      <c r="D115" t="s">
         <v>226</v>
-      </c>
-      <c r="C115" t="s">
-        <v>219</v>
-      </c>
-      <c r="D115" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -6636,13 +6682,13 @@
         <v>10</v>
       </c>
       <c r="B116" t="s">
+        <v>227</v>
+      </c>
+      <c r="C116" t="s">
+        <v>26</v>
+      </c>
+      <c r="D116" t="s">
         <v>228</v>
-      </c>
-      <c r="C116" t="s">
-        <v>27</v>
-      </c>
-      <c r="D116" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -6650,16 +6696,16 @@
         <v>11</v>
       </c>
       <c r="B117" t="s">
+        <v>229</v>
+      </c>
+      <c r="C117" t="s">
+        <v>26</v>
+      </c>
+      <c r="D117" t="s">
+        <v>340</v>
+      </c>
+      <c r="E117" t="s">
         <v>230</v>
-      </c>
-      <c r="C117" t="s">
-        <v>27</v>
-      </c>
-      <c r="D117" t="s">
-        <v>341</v>
-      </c>
-      <c r="E117" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -6667,10 +6713,10 @@
         <v>10</v>
       </c>
       <c r="B118" t="s">
+        <v>231</v>
+      </c>
+      <c r="C118" t="s">
         <v>232</v>
-      </c>
-      <c r="C118" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -6678,13 +6724,13 @@
         <v>8</v>
       </c>
       <c r="B119" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C119" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D119" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -6692,16 +6738,16 @@
         <v>9</v>
       </c>
       <c r="B120" t="s">
+        <v>366</v>
+      </c>
+      <c r="C120" t="s">
+        <v>26</v>
+      </c>
+      <c r="D120" t="s">
         <v>367</v>
       </c>
-      <c r="C120" t="s">
-        <v>27</v>
-      </c>
-      <c r="D120" t="s">
-        <v>368</v>
-      </c>
       <c r="E120" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -6709,10 +6755,10 @@
         <v>10</v>
       </c>
       <c r="B121" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="C121" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -6720,13 +6766,13 @@
         <v>7</v>
       </c>
       <c r="B122" t="s">
+        <v>234</v>
+      </c>
+      <c r="C122" t="s">
         <v>235</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
         <v>236</v>
-      </c>
-      <c r="D122" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -6734,10 +6780,10 @@
         <v>8</v>
       </c>
       <c r="B123" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C123" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -6745,10 +6791,10 @@
         <v>0</v>
       </c>
       <c r="B124" t="s">
+        <v>39</v>
+      </c>
+      <c r="D124" t="s">
         <v>40</v>
-      </c>
-      <c r="D124" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -6756,13 +6802,13 @@
         <v>1</v>
       </c>
       <c r="B125" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C125" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D125" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -6770,10 +6816,10 @@
         <v>2</v>
       </c>
       <c r="B126" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C126" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D126" t="s">
         <v>0</v>
@@ -6784,13 +6830,13 @@
         <v>3</v>
       </c>
       <c r="B127" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C127" t="b">
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -6798,13 +6844,13 @@
         <v>4</v>
       </c>
       <c r="B128" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C128" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D128" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -6812,10 +6858,10 @@
         <v>5</v>
       </c>
       <c r="B129" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C129" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D129" t="s">
         <v>2</v>
@@ -6826,10 +6872,10 @@
         <v>6</v>
       </c>
       <c r="B130" t="s">
+        <v>242</v>
+      </c>
+      <c r="C130" t="s">
         <v>243</v>
-      </c>
-      <c r="C130" t="s">
-        <v>244</v>
       </c>
       <c r="D130" t="s">
         <v>3</v>
@@ -6840,10 +6886,10 @@
         <v>7</v>
       </c>
       <c r="B131" t="s">
+        <v>244</v>
+      </c>
+      <c r="C131" t="s">
         <v>245</v>
-      </c>
-      <c r="C131" t="s">
-        <v>246</v>
       </c>
       <c r="D131" t="s">
         <v>4</v>
@@ -6854,16 +6900,16 @@
         <v>8</v>
       </c>
       <c r="B132" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C132" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D132" t="s">
         <v>5</v>
       </c>
       <c r="E132" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -6871,13 +6917,13 @@
         <v>9</v>
       </c>
       <c r="B133" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C133" t="b">
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -6885,13 +6931,13 @@
         <v>10</v>
       </c>
       <c r="B134" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C134" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D134" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -6899,7 +6945,7 @@
         <v>11</v>
       </c>
       <c r="B135" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C135" t="b">
         <v>1</v>
@@ -6910,7 +6956,7 @@
         <v>11</v>
       </c>
       <c r="B136" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C136" t="b">
         <v>0</v>
@@ -6921,7 +6967,7 @@
         <v>9</v>
       </c>
       <c r="B137" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C137" t="b">
         <v>0</v>
@@ -6935,10 +6981,10 @@
         <v>10</v>
       </c>
       <c r="B138" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="C138" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -6946,10 +6992,10 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C139" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D139" t="s">
         <v>7</v>
@@ -6960,10 +7006,10 @@
         <v>8</v>
       </c>
       <c r="B140" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C140" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -6971,10 +7017,10 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
+        <v>253</v>
+      </c>
+      <c r="C141" t="s">
         <v>254</v>
-      </c>
-      <c r="C141" t="s">
-        <v>255</v>
       </c>
       <c r="D141" t="s">
         <v>1</v>
@@ -6985,13 +7031,13 @@
         <v>8</v>
       </c>
       <c r="B142" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="C142" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D142" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -6999,7 +7045,7 @@
         <v>9</v>
       </c>
       <c r="B143" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="C143" t="b">
         <v>1</v>
@@ -7010,13 +7056,13 @@
         <v>9</v>
       </c>
       <c r="B144" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C144" t="b">
         <v>0</v>
       </c>
       <c r="D144" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -7024,13 +7070,13 @@
         <v>10</v>
       </c>
       <c r="B145" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C145" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D145" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -7038,10 +7084,10 @@
         <v>11</v>
       </c>
       <c r="B146" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C146" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -7049,10 +7095,10 @@
         <v>6</v>
       </c>
       <c r="B147" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C147" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -7060,10 +7106,10 @@
         <v>6</v>
       </c>
       <c r="B148" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C148" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -7071,7 +7117,7 @@
         <v>5</v>
       </c>
       <c r="B149" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C149" t="b">
         <v>1</v>
@@ -7085,13 +7131,13 @@
         <v>6</v>
       </c>
       <c r="B150" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C150" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D150" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -7099,10 +7145,10 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
+        <v>260</v>
+      </c>
+      <c r="C151" t="s">
         <v>261</v>
-      </c>
-      <c r="C151" t="s">
-        <v>262</v>
       </c>
       <c r="D151" t="s">
         <v>9</v>
@@ -7113,10 +7159,10 @@
         <v>8</v>
       </c>
       <c r="B152" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C152" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D152" t="s">
         <v>10</v>
@@ -7127,13 +7173,13 @@
         <v>9</v>
       </c>
       <c r="B153" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C153" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D153" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -7141,13 +7187,13 @@
         <v>10</v>
       </c>
       <c r="B154" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C154" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D154" t="s">
-        <v>11</v>
+        <v>418</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -7155,13 +7201,13 @@
         <v>7</v>
       </c>
       <c r="B155" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C155" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D155" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -7169,10 +7215,10 @@
         <v>8</v>
       </c>
       <c r="B156" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C156" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -7180,10 +7226,10 @@
         <v>4</v>
       </c>
       <c r="B157" t="s">
+        <v>267</v>
+      </c>
+      <c r="C157" t="s">
         <v>268</v>
-      </c>
-      <c r="C157" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -7191,16 +7237,16 @@
         <v>4</v>
       </c>
       <c r="B158" t="s">
+        <v>269</v>
+      </c>
+      <c r="C158" t="s">
         <v>270</v>
       </c>
-      <c r="C158" t="s">
-        <v>271</v>
-      </c>
       <c r="D158" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E158" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -7208,10 +7254,10 @@
         <v>5</v>
       </c>
       <c r="B159" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C159" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -7219,13 +7265,13 @@
         <v>3</v>
       </c>
       <c r="B160" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C160" t="b">
         <v>0</v>
       </c>
       <c r="D160" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="161" spans="1:4">
@@ -7233,13 +7279,13 @@
         <v>4</v>
       </c>
       <c r="B161" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C161" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D161" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="162" spans="1:4">
@@ -7247,10 +7293,10 @@
         <v>5</v>
       </c>
       <c r="B162" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C162" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D162" t="s">
         <v>8</v>
@@ -7261,13 +7307,13 @@
         <v>6</v>
       </c>
       <c r="B163" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C163" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D163" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="164" spans="1:4">
@@ -7275,13 +7321,13 @@
         <v>7</v>
       </c>
       <c r="B164" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C164" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D164" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="165" spans="1:4">
@@ -7289,13 +7335,13 @@
         <v>8</v>
       </c>
       <c r="B165" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C165" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D165" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="166" spans="1:4">
@@ -7303,7 +7349,7 @@
         <v>9</v>
       </c>
       <c r="B166" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C166" t="b">
         <v>1</v>
@@ -7314,13 +7360,13 @@
         <v>9</v>
       </c>
       <c r="B167" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C167" t="b">
         <v>0</v>
       </c>
       <c r="D167" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="168" spans="1:4">
@@ -7328,10 +7374,10 @@
         <v>10</v>
       </c>
       <c r="B168" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C168" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="169" spans="1:4">
@@ -7339,10 +7385,10 @@
         <v>9</v>
       </c>
       <c r="B169" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C169" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="170" spans="1:4">
@@ -7350,13 +7396,13 @@
         <v>7</v>
       </c>
       <c r="B170" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C170" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D170" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="171" spans="1:4">
@@ -7364,13 +7410,13 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C171" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D171" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="172" spans="1:4">
@@ -7378,10 +7424,10 @@
         <v>9</v>
       </c>
       <c r="B172" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C172" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="173" spans="1:4">
@@ -7389,7 +7435,7 @@
         <v>5</v>
       </c>
       <c r="B173" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C173" t="b">
         <v>0</v>
@@ -7403,10 +7449,10 @@
         <v>6</v>
       </c>
       <c r="B174" t="s">
+        <v>242</v>
+      </c>
+      <c r="C174" t="s">
         <v>243</v>
-      </c>
-      <c r="C174" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="175" spans="1:4">
@@ -7414,10 +7460,10 @@
         <v>6</v>
       </c>
       <c r="B175" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C175" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="176" spans="1:4">
@@ -7425,10 +7471,10 @@
         <v>6</v>
       </c>
       <c r="B176" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C176" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -7436,10 +7482,10 @@
         <v>4</v>
       </c>
       <c r="B177" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C177" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D177" t="s">
         <v>6</v>
@@ -7450,10 +7496,10 @@
         <v>5</v>
       </c>
       <c r="B178" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C178" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -7461,7 +7507,7 @@
         <v>5</v>
       </c>
       <c r="B179" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C179" t="b">
         <v>0</v>
@@ -7472,10 +7518,10 @@
         <v>4</v>
       </c>
       <c r="B180" t="s">
+        <v>269</v>
+      </c>
+      <c r="C180" t="s">
         <v>270</v>
-      </c>
-      <c r="C180" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -7483,10 +7529,10 @@
         <v>3</v>
       </c>
       <c r="B181" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C181" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D181" t="s">
         <v>4</v>
@@ -7497,13 +7543,13 @@
         <v>4</v>
       </c>
       <c r="B182" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C182" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D182" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -7511,13 +7557,13 @@
         <v>5</v>
       </c>
       <c r="B183" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C183" t="b">
         <v>1</v>
       </c>
       <c r="D183" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -7525,10 +7571,10 @@
         <v>6</v>
       </c>
       <c r="B184" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C184" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D184" t="s">
         <v>6</v>
@@ -7539,10 +7585,10 @@
         <v>7</v>
       </c>
       <c r="B185" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C185" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -7550,7 +7596,7 @@
         <v>7</v>
       </c>
       <c r="B186" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C186" t="b">
         <v>1</v>
@@ -7561,10 +7607,10 @@
         <v>6</v>
       </c>
       <c r="B187" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C187" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -7572,7 +7618,7 @@
         <v>5</v>
       </c>
       <c r="B188" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="C188" t="b">
         <v>0</v>
@@ -7583,13 +7629,13 @@
         <v>5</v>
       </c>
       <c r="B189" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C189" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D189" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -7597,16 +7643,16 @@
         <v>6</v>
       </c>
       <c r="B190" t="s">
+        <v>296</v>
+      </c>
+      <c r="C190" t="s">
+        <v>254</v>
+      </c>
+      <c r="D190" t="s">
         <v>297</v>
       </c>
-      <c r="C190" t="s">
-        <v>255</v>
-      </c>
-      <c r="D190" t="s">
-        <v>298</v>
-      </c>
       <c r="E190" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -7614,7 +7660,7 @@
         <v>7</v>
       </c>
       <c r="B191" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C191" t="b">
         <v>1</v>
@@ -7625,7 +7671,7 @@
         <v>7</v>
       </c>
       <c r="B192" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C192" t="b">
         <v>0</v>
@@ -7636,16 +7682,16 @@
         <v>6</v>
       </c>
       <c r="B193" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C193" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D193" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E193" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -7653,7 +7699,7 @@
         <v>7</v>
       </c>
       <c r="B194" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C194" t="b">
         <v>1</v>
@@ -7664,7 +7710,7 @@
         <v>7</v>
       </c>
       <c r="B195" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C195" t="b">
         <v>0</v>
@@ -7675,13 +7721,13 @@
         <v>0</v>
       </c>
       <c r="B196" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D196" t="s">
+        <v>371</v>
+      </c>
+      <c r="E196" t="s">
         <v>372</v>
-      </c>
-      <c r="E196" t="s">
-        <v>373</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -7689,13 +7735,13 @@
         <v>1</v>
       </c>
       <c r="B197" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="C197" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D197" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -7703,13 +7749,13 @@
         <v>2</v>
       </c>
       <c r="B198" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C198" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D198" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -7717,13 +7763,13 @@
         <v>3</v>
       </c>
       <c r="B199" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C199" t="b">
         <v>1</v>
       </c>
       <c r="D199" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -7731,13 +7777,13 @@
         <v>4</v>
       </c>
       <c r="B200" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="C200" t="b">
         <v>0</v>
       </c>
       <c r="D200" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -7745,10 +7791,10 @@
         <v>5</v>
       </c>
       <c r="B201" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C201" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -7756,7 +7802,7 @@
         <v>4</v>
       </c>
       <c r="B202" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C202" t="b">
         <v>1</v>
@@ -7767,13 +7813,13 @@
         <v>3</v>
       </c>
       <c r="B203" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="C203" t="b">
         <v>0</v>
       </c>
       <c r="D203" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -7781,13 +7827,13 @@
         <v>4</v>
       </c>
       <c r="B204" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C204" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D204" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -7795,13 +7841,13 @@
         <v>5</v>
       </c>
       <c r="B205" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C205" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D205" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -7809,16 +7855,16 @@
         <v>6</v>
       </c>
       <c r="B206" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C206" t="b">
         <v>0</v>
       </c>
       <c r="D206" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E206" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -7826,13 +7872,13 @@
         <v>7</v>
       </c>
       <c r="B207" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C207" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D207" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -7840,13 +7886,13 @@
         <v>8</v>
       </c>
       <c r="B208" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C208" t="b">
         <v>1</v>
       </c>
       <c r="D208" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -7854,7 +7900,7 @@
         <v>9</v>
       </c>
       <c r="B209" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C209" t="b">
         <v>0</v>
@@ -7865,7 +7911,7 @@
         <v>9</v>
       </c>
       <c r="B210" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C210" t="b">
         <v>1</v>
@@ -7876,13 +7922,13 @@
         <v>8</v>
       </c>
       <c r="B211" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C211" t="b">
         <v>0</v>
       </c>
       <c r="D211" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -7890,13 +7936,13 @@
         <v>9</v>
       </c>
       <c r="B212" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C212" t="b">
         <v>1</v>
       </c>
       <c r="D212" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -7904,10 +7950,10 @@
         <v>10</v>
       </c>
       <c r="B213" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C213" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -7915,13 +7961,13 @@
         <v>9</v>
       </c>
       <c r="B214" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C214" t="b">
         <v>0</v>
       </c>
       <c r="D214" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="215" spans="1:5">
@@ -7929,10 +7975,10 @@
         <v>10</v>
       </c>
       <c r="B215" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C215" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -7940,7 +7986,7 @@
         <v>6</v>
       </c>
       <c r="B216" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C216" t="b">
         <v>1</v>
@@ -7954,13 +8000,13 @@
         <v>7</v>
       </c>
       <c r="B217" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C217" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D217" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -7968,7 +8014,7 @@
         <v>8</v>
       </c>
       <c r="B218" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C218" t="b">
         <v>0</v>
@@ -7979,7 +8025,7 @@
         <v>8</v>
       </c>
       <c r="B219" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C219" t="b">
         <v>1</v>
@@ -7990,13 +8036,13 @@
         <v>5</v>
       </c>
       <c r="B220" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C220" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D220" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -8004,7 +8050,7 @@
         <v>6</v>
       </c>
       <c r="B221" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C221" t="b">
         <v>0</v>
@@ -8015,7 +8061,7 @@
         <v>6</v>
       </c>
       <c r="B222" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="C222" t="b">
         <v>1</v>
@@ -8026,16 +8072,16 @@
         <v>1</v>
       </c>
       <c r="B223" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C223" t="b">
         <v>1</v>
       </c>
       <c r="D223" t="s">
+        <v>373</v>
+      </c>
+      <c r="E223" t="s">
         <v>374</v>
-      </c>
-      <c r="E223" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="224" spans="1:5">
@@ -8043,18 +8089,18 @@
         <v>2</v>
       </c>
       <c r="B224" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C224" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D224" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="225" spans="1:6">
       <c r="A225" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="226" spans="1:6">
@@ -8062,13 +8108,13 @@
         <v>0</v>
       </c>
       <c r="B226" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D226" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E226" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
     </row>
     <row r="227" spans="1:6">
@@ -8076,19 +8122,19 @@
         <v>1</v>
       </c>
       <c r="B227" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="C227" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D227" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E227" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F227" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -8096,13 +8142,13 @@
         <v>2</v>
       </c>
       <c r="B228" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C228" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D228" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="229" spans="1:6">
@@ -8110,13 +8156,13 @@
         <v>3</v>
       </c>
       <c r="B229" t="s">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="C229" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D229" t="s">
-        <v>396</v>
+        <v>391</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -8124,13 +8170,13 @@
         <v>4</v>
       </c>
       <c r="B230" t="s">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="C230" t="b">
         <v>1</v>
       </c>
       <c r="D230" t="s">
-        <v>399</v>
+        <v>394</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -8138,13 +8184,13 @@
         <v>5</v>
       </c>
       <c r="B231" t="s">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C231" t="b">
         <v>0</v>
       </c>
       <c r="D231" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="232" spans="1:6">
@@ -8152,10 +8198,10 @@
         <v>6</v>
       </c>
       <c r="B232" t="s">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="C232" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="233" spans="1:6">
@@ -8163,7 +8209,7 @@
         <v>5</v>
       </c>
       <c r="B233" t="s">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="C233" t="b">
         <v>1</v>
@@ -8174,13 +8220,13 @@
         <v>4</v>
       </c>
       <c r="B234" t="s">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="C234" t="b">
         <v>0</v>
       </c>
       <c r="D234" t="s">
-        <v>404</v>
+        <v>399</v>
       </c>
     </row>
     <row r="235" spans="1:6">
@@ -8188,13 +8234,13 @@
         <v>5</v>
       </c>
       <c r="B235" t="s">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="C235" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D235" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -8202,13 +8248,13 @@
         <v>6</v>
       </c>
       <c r="B236" t="s">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="C236" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D236" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -8216,16 +8262,16 @@
         <v>7</v>
       </c>
       <c r="B237" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C237" t="b">
         <v>0</v>
       </c>
       <c r="D237" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E237" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -8233,13 +8279,13 @@
         <v>8</v>
       </c>
       <c r="B238" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C238" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D238" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -8247,13 +8293,13 @@
         <v>9</v>
       </c>
       <c r="B239" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C239" t="b">
         <v>1</v>
       </c>
       <c r="D239" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -8261,7 +8307,7 @@
         <v>10</v>
       </c>
       <c r="B240" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="C240" t="b">
         <v>0</v>
@@ -8272,7 +8318,7 @@
         <v>10</v>
       </c>
       <c r="B241" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="C241" t="b">
         <v>1</v>
@@ -8283,13 +8329,13 @@
         <v>9</v>
       </c>
       <c r="B242" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="C242" t="b">
         <v>0</v>
       </c>
       <c r="D242" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
     </row>
     <row r="243" spans="1:4">
@@ -8297,13 +8343,13 @@
         <v>10</v>
       </c>
       <c r="B243" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="C243" t="b">
         <v>1</v>
       </c>
       <c r="D243" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="244" spans="1:4">
@@ -8311,10 +8357,10 @@
         <v>11</v>
       </c>
       <c r="B244" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C244" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="245" spans="1:4">
@@ -8322,13 +8368,13 @@
         <v>10</v>
       </c>
       <c r="B245" t="s">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="C245" t="b">
         <v>0</v>
       </c>
       <c r="D245" t="s">
-        <v>397</v>
+        <v>392</v>
       </c>
     </row>
     <row r="246" spans="1:4">
@@ -8336,10 +8382,10 @@
         <v>11</v>
       </c>
       <c r="B246" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="C246" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="247" spans="1:4">
@@ -8347,7 +8393,7 @@
         <v>7</v>
       </c>
       <c r="B247" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C247" t="b">
         <v>1</v>
@@ -8361,13 +8407,13 @@
         <v>8</v>
       </c>
       <c r="B248" t="s">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="C248" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D248" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
     </row>
     <row r="249" spans="1:4">
@@ -8375,7 +8421,7 @@
         <v>9</v>
       </c>
       <c r="B249" t="s">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="C249" t="b">
         <v>0</v>
@@ -8386,7 +8432,7 @@
         <v>9</v>
       </c>
       <c r="B250" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="C250" t="b">
         <v>1</v>
@@ -8397,13 +8443,13 @@
         <v>6</v>
       </c>
       <c r="B251" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="C251" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D251" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="252" spans="1:4">
@@ -8411,7 +8457,7 @@
         <v>7</v>
       </c>
       <c r="B252" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="C252" t="b">
         <v>0</v>
@@ -8422,7 +8468,7 @@
         <v>7</v>
       </c>
       <c r="B253" t="s">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="C253" t="b">
         <v>1</v>
@@ -8433,13 +8479,13 @@
         <v>2</v>
       </c>
       <c r="B254" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C254" t="b">
         <v>1</v>
       </c>
       <c r="D254" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
     </row>
     <row r="255" spans="1:4">
@@ -8447,13 +8493,13 @@
         <v>3</v>
       </c>
       <c r="B255" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C255" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D255" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="256" spans="1:4">
@@ -8461,38 +8507,74 @@
         <v>0</v>
       </c>
       <c r="B256" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D256" t="s">
-        <v>389</v>
-      </c>
-    </row>
-    <row r="257" spans="1:5">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="257" spans="1:4">
       <c r="A257">
         <v>1</v>
       </c>
       <c r="B257" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="C257" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D257" t="s">
-        <v>394</v>
-      </c>
-      <c r="E257" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="258" spans="1:5">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="258" spans="1:4">
       <c r="A258">
         <v>2</v>
       </c>
       <c r="B258" t="s">
-        <v>390</v>
+        <v>422</v>
       </c>
       <c r="C258" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D258" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="259" spans="1:4">
+      <c r="A259">
+        <v>3</v>
+      </c>
+      <c r="B259" t="s">
+        <v>425</v>
+      </c>
+      <c r="C259" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="260" spans="1:4">
+      <c r="A260">
+        <v>2</v>
+      </c>
+      <c r="B260" t="s">
+        <v>421</v>
+      </c>
+      <c r="C260" t="b">
+        <v>1</v>
+      </c>
+      <c r="D260" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="261" spans="1:4">
+      <c r="A261">
+        <v>3</v>
+      </c>
+      <c r="B261" t="s">
+        <v>425</v>
+      </c>
+      <c r="C261" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added performance level guide
- On “test record select” prompt, show a list of performances possible.
</commit_message>
<xml_diff>
--- a/auto-agent/workflow.xlsx
+++ b/auto-agent/workflow.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="498">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1883" uniqueCount="501">
   <si>
     <t>Ok, I see. Based on the chart, you think that people who have {{$factor := index .ContentFactors .TargetFactor.FactorId}}{{$bestlevel := index $factor.Levels 0}}{{$bestlevel.Text}} and those who have {{$alevel := index $factor.Levels 1}}{{$alevel.Text}} for {{.TargetFactor.FactorName}} have the same performance.</t>
   </si>
@@ -1515,6 +1515,15 @@
   </si>
   <si>
     <t>Now, Suppose someone disagrees with you and thinks that {{.TargetFactor.FactorName}} really does make a difference to performance in space. What would you say to them?</t>
+  </si>
+  <si>
+    <t>I have a list of records about the applicants. If you study them carefully, you can see which factors matter to performance and which don't.</t>
+  </si>
+  <si>
+    <t>Let's try it. On the screen, you can find any applicant to look at. Just select a level for each factor, and the computer will find you an applicant with those levels and tell you his/her performance.</t>
+  </si>
+  <si>
+    <t>You selected Record #{{.RecordNoOne.RecordNo}}, {{.RecordNoOne.RecordName}}. You can see that performance can be from A to E. And {{.RecordNoOne.FirstName}}'s performance was {{.RecordNoOne.Performance}}.</t>
   </si>
 </sst>
 </file>
@@ -1563,8 +1572,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2171">
+  <cellStyleXfs count="2173">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -3739,7 +3750,7 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="2171">
+  <cellStyles count="2173">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -4825,6 +4836,7 @@
     <cellStyle name="Followed Hyperlink" xfId="2166" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2168" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="2170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="2172" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -5910,6 +5922,7 @@
     <cellStyle name="Hyperlink" xfId="2165" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2167" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2171" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -6241,8 +6254,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H281"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6349,10 +6362,10 @@
         <v>371</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>498</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>499</v>
       </c>
       <c r="H6" t="s">
         <v>33</v>
@@ -6372,7 +6385,7 @@
         <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>35</v>
+        <v>500</v>
       </c>
       <c r="G7" t="s">
         <v>36</v>
@@ -10711,6 +10724,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>